<commit_message>
Feeder setup Page Done
</commit_message>
<xml_diff>
--- a/Files/Feeder Setup   16_05_2023.xlsx
+++ b/Files/Feeder Setup   16_05_2023.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="MX2CDCCAQ600C00-F303" sheetId="2" r:id="R4691fe03f34f4520"/>
+    <x:sheet name="MX2CDCCAQ600C00-F303" sheetId="2" r:id="R6085245db7aa4d79"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -86,6 +86,468 @@
     <x:t>M5401-23050001</x:t>
   </x:si>
   <x:si>
+    <x:t>01S1001K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S1001K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">150  </x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R811, 9:R811, 8:R811, 7:R811, 6:R811, 5:R811, 4:R811, 3:R811, 2:R811, 1:R811, 10:R809, 9:R809, 8:R809, 7:R809, 6:R809, 5:R809, 4:R809, 3:R809, 2:R809, 1:R809, 10:R806, 9:R806, 8:R806, 7:R806, 6:R806, 5:R806, 4:R806, 3:R806, 2:R806, 1:R806, 10:R844, 9:R844, 8:R844, 7:R844, 6:R844, 5:R844, 4:R844, 3:R844, 2:R844, 1:R844, 10:R849, 9:R849, 8:R849, 7:R849, 6:R849, 5:R849, 4:R849, 3:R849, 2:R849, 1:R849, 11:R811, 12:R811, 13:R811, 14:R811, 15:R811, 16:R811, 17:R811, 18:R811, 19:R811, 20:R811, 11:R809, 12:R809, 13:R809, 14:R809, 15:R809, 16:R809, 17:R809, 18:R809, 19:R809, 20:R809, 11:R806, 12:R806, 13:R806, 14:R806, 15:R806, 16:R806, 17:R806, 18:R806, 19:R806, 20:R806, 11:R844, 12:R844, 13:R844, 14:R844, 15:R844, 16:R844, 17:R844, 18:R844, 19:R844, 20:R844, 11:R849, 12:R849, 13:R849, 14:R849, 15:R849, 16:R849, 17:R849, 18:R849, 19:R849, 20:R849, 30:R811, 29:R811, 28:R811, 27:R811, 26:R811, 25:R811, 24:R811, 23:R811, 22:R811, 21:R811, 30:R809, 29:R809, 28:R809, 27:R809, 26:R809, 25:R809, 24:R809, 23:R809, 22:R809, 21:R809, 30:R806, 29:R806, 28:R806, 27:R806, 26:R806, 25:R806, 24:R806, 23:R806, 22:R806, 21:R806, 30:R844, 29:R844, 28:R844, 27:R844, 26:R844, 25:R844, 24:R844, 23:R844, 22:R844, 21:R844, 30:R849, 29:R849, 28:R849, 27:R849, 26:R849, 25:R849, 24:R849, 23:R849, 22:R849, 21:R849,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KT-0800F-180</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1- 20    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">20   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bottom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>02S1050001-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30302S1050001-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">60   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:C807, 9:C807, 8:C807, 7:C807, 6:C807, 5:C807, 4:C807, 3:C807, 2:C807, 1:C807, 10:C808, 9:C808, 8:C808, 7:C808, 6:C808, 5:C808, 4:C808, 3:C808, 2:C808, 1:C808, 11:C807, 12:C807, 13:C807, 14:C807, 15:C807, 16:C807, 17:C807, 18:C807, 19:C807, 20:C807, 11:C808, 12:C808, 13:C808, 14:C808, 15:C808, 16:C808, 17:C808, 18:C808, 19:C808, 20:C808, 30:C807, 29:C807, 28:C807, 27:C807, 26:C807, 25:C807, 24:C807, 23:C807, 22:C807, 21:C807, 30:C808, 29:C808, 28:C808, 27:C808, 26:C808, 25:C808, 24:C808, 23:C808, 22:C808, 21:C808,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1- 21    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">21   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S3302K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S3302K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">30   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R818, 9:R818, 8:R818, 7:R818, 6:R818, 5:R818, 4:R818, 3:R818, 2:R818, 1:R818, 11:R818, 12:R818, 13:R818, 14:R818, 15:R818, 16:R818, 17:R818, 18:R818, 19:R818, 20:R818, 30:R818, 29:R818, 28:R818, 27:R818, 26:R818, 25:R818, 24:R818, 23:R818, 22:R818, 21:R818,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1- 22    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">22   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S6800K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S6800K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R815, 9:R815, 8:R815, 7:R815, 6:R815, 5:R815, 4:R815, 3:R815, 2:R815, 1:R815, 10:R824, 9:R824, 8:R824, 7:R824, 6:R824, 5:R824, 4:R824, 3:R824, 2:R824, 1:R824, 11:R815, 12:R815, 13:R815, 14:R815, 15:R815, 16:R815, 17:R815, 18:R815, 19:R815, 20:R815, 11:R824, 12:R824, 13:R824, 14:R824, 15:R824, 16:R824, 17:R824, 18:R824, 19:R824, 20:R824, 30:R815, 29:R815, 28:R815, 27:R815, 26:R815, 25:R815, 24:R815, 23:R815, 22:R815, 21:R815, 30:R824, 29:R824, 28:R824, 26:R824, 27:R824, 25:R824, 24:R824, 23:R824, 22:R824, 21:R824,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1- 24    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">24   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S1003K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S1003K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">90   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R842, 9:R842, 8:R842, 7:R842, 6:R842, 5:R842, 4:R842, 3:R842, 2:R842, 1:R842, 10:R839, 9:R839, 8:R839, 7:R839, 6:R839, 5:R839, 4:R839, 3:R839, 2:R839, 1:R839, 10:R836, 9:R836, 8:R836, 7:R836, 6:R836, 5:R836, 4:R836, 3:R836, 2:R836, 1:R836, 11:R842, 12:R842, 13:R842, 14:R842, 15:R842, 16:R842, 17:R842, 18:R842, 19:R842, 20:R842, 11:R839, 12:R839, 13:R839, 14:R839, 15:R839, 16:R839, 17:R839, 18:R839, 19:R839, 20:R839, 11:R836, 12:R836, 13:R836, 14:R836, 15:R836, 16:R836, 17:R836, 18:R836, 19:R836, 20:R836, 30:R842, 29:R842, 28:R842, 27:R842, 26:R842, 25:R842, 24:R842, 23:R842, 22:R842, 21:R842, 30:R839, 29:R839, 28:R839, 27:R839, 26:R839, 25:R839, 24:R839, 23:R839, 22:R839, 21:R839, 30:R836, 29:R836, 28:R836, 27:R836, 26:R836, 25:R836, 24:R836, 23:R836, 22:R836, 21:R836,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1- 25    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">25   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S5101K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S5101K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R820, 10:R822, 9:R820, 9:R822, 8:R820, 8:R822, 7:R820, 7:R822, 6:R820, 6:R822, 5:R820, 5:R822, 4:R820, 4:R822, 3:R820, 3:R822, 2:R820, 2:R822, 1:R820, 1:R822, 11:R820, 11:R822, 12:R820, 12:R822, 13:R820, 13:R822, 14:R820, 14:R822, 15:R820, 15:R822, 16:R820, 16:R822, 17:R820, 17:R822, 18:R820, 18:R822, 19:R820, 19:R822, 20:R820, 20:R822, 30:R820, 30:R822, 29:R820, 29:R822, 28:R820, 28:R822, 27:R820, 27:R822, 26:R820, 26:R822, 25:R820, 25:R822, 24:R820, 24:R822, 23:R820, 23:R822, 22:R820, 22:R822, 21:R820, 21:R822,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1- 26    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">26   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S1002310-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S1002310-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R833, 9:R833, 8:R833, 7:R833, 6:R833, 5:R833, 4:R833, 3:R833, 2:R833, 1:R833, 20:R833, 19:R833, 18:R833, 17:R833, 16:R833, 15:R833, 14:R833, 13:R833, 12:R833, 11:R833, 30:R833, 29:R833, 28:R833, 27:R833, 26:R833, 25:R833, 24:R833, 23:R833, 22:R833, 21:R833,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 14    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">14   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S5102K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S5102K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R805, 9:R805, 8:R805, 7:R805, 6:R805, 5:R805, 4:R805, 3:R805, 2:R805, 1:R805, 20:R805, 19:R805, 18:R805, 17:R805, 16:R805, 15:R805, 14:R805, 13:R805, 12:R805, 11:R805, 30:R805, 29:R805, 28:R805, 27:R805, 26:R805, 25:R805, 24:R805, 23:R805, 22:R805, 21:R805,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 20    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S1002K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S1002K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R846, 9:R846, 8:R846, 7:R846, 6:R846, 5:R846, 4:R846, 3:R846, 2:R846, 1:R846, 20:R846, 19:R846, 18:R846, 17:R846, 16:R846, 15:R846, 14:R846, 13:R846, 12:R846, 11:R846, 30:R846, 29:R846, 28:R846, 27:R846, 26:R846, 25:R846, 24:R846, 23:R846, 22:R846, 21:R846,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 22    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>02S1040201-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30302S1040201-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">180  </x:t>
+  </x:si>
+  <x:si>
+    <x:t>20:C813, 20:C817, 21:C804, 21:C805, 21:C803, 21:C818, 21:C813, 21:C817, 22:C817, 22:C813, 22:C818, 22:C803, 22:C805, 22:C804, 19:C817, 19:C813, 18:C813, 18:C817, 24:C804, 24:C805, 24:C803, 24:C818, 23:C804, 23:C805, 23:C803, 23:C818, 23:C813, 23:C817, 24:C813, 24:C817, 25:C817, 25:C813, 25:C818, 25:C803, 25:C805, 25:C804, 16:C817, 16:C813, 17:C817, 17:C813, 17:C818, 17:C803, 17:C805, 17:C804, 16:C818, 16:C803, 16:C805, 16:C804, 4:C817, 4:C813, 3:C813, 3:C817, 18:C804, 18:C805, 18:C803, 18:C818, 19:C804, 19:C805, 19:C803, 19:C818, 20:C803, 20:C805, 20:C818, 20:C804, 1:C817, 1:C813, 1:C818, 1:C803, 1:C805, 1:C804, 2:C804, 2:C805, 2:C803, 2:C818, 2:C813, 2:C817, 3:C818, 3:C803, 3:C805, 3:C804, 4:C818, 4:C803, 4:C805, 4:C804, 5:C804, 5:C805, 5:C803, 5:C818, 5:C813, 5:C817, 6:C803, 6:C805, 6:C804, 6:C818, 6:C813, 6:C817, 7:C817, 7:C813, 7:C818, 7:C803, 7:C805, 7:C804, 8:C818, 8:C804, 8:C805, 8:C803, 8:C813, 8:C817, 9:C818, 9:C803, 9:C805, 9:C804, 10:C804, 10:C805, 10:C803, 10:C818, 10:C813, 10:C817, 9:C813, 9:C817, 11:C804, 11:C805, 11:C803, 11:C818, 12:C804, 12:C805, 12:C803, 12:C818, 13:C817, 13:C813, 13:C818, 13:C803, 13:C805, 13:C804, 14:C804, 14:C805, 14:C803, 14:C818, 15:C804, 15:C805, 15:C803, 15:C818, 15:C813, 15:C817, 26:C804, 26:C805, 26:C803, 26:C818, 26:C813, 26:C817, 27:C817, 27:C813, 27:C818, 27:C803, 27:C805, 27:C804, 14:C817, 14:C813, 28:C803, 28:C805, 28:C818, 28:C804, 29:C818, 29:C803, 29:C805, 29:C804, 12:C817, 12:C813, 11:C813, 11:C817, 30:C804, 30:C805, 30:C803, 30:C818, 30:C813, 30:C817, 29:C817, 29:C813, 28:C817, 28:C813,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 23    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">23   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S2001K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S2001K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23:R840, 24:R840, 25:R840, 26:R840, 27:R840, 28:R840, 29:R840, 30:R840, 30:R812, 30:R813, 11:R840, 11:R812, 11:R813, 12:R812, 12:R813, 13:R812, 13:R813, 12:R840, 29:R812, 29:R813, 28:R812, 28:R813, 13:R840, 27:R812, 27:R813, 14:R840, 14:R812, 14:R813, 15:R812, 15:R813, 16:R812, 16:R813, 15:R840, 26:R812, 26:R813, 25:R812, 25:R813, 16:R840, 24:R812, 24:R813, 23:R812, 23:R813, 22:R812, 22:R813, 18:R840, 17:R840, 17:R812, 17:R813, 18:R812, 18:R813, 19:R812, 19:R813, 3:R840, 4:R840, 5:R840, 6:R840, 7:R840, 8:R840, 9:R840, 10:R840, 10:R812, 10:R813, 9:R812, 9:R813, 8:R812, 8:R813, 7:R812, 7:R813, 6:R812, 6:R813, 5:R812, 5:R813, 4:R812, 4:R813, 3:R812, 3:R813, 2:R812, 2:R813, 1:R812, 1:R813, 2:R840, 1:R840, 20:R812, 20:R813, 19:R840, 20:R840, 21:R812, 21:R813, 22:R840, 21:R840,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 24    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S2002K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S2002K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21:R838, 21:R832, 21:R834, 22:R838, 22:R834, 22:R832, 23:R838, 23:R832, 23:R834, 24:R838, 24:R834, 24:R832, 25:R838, 25:R834, 25:R832, 26:R838, 26:R834, 26:R832, 27:R838, 27:R834, 27:R832, 28:R838, 28:R834, 28:R832, 29:R838, 29:R834, 29:R832, 30:R838, 30:R834, 30:R832, 11:R834, 11:R832, 11:R838, 12:R834, 12:R832, 12:R838, 13:R832, 13:R834, 13:R838, 14:R832, 14:R834, 14:R838, 15:R832, 15:R834, 15:R838, 16:R832, 16:R834, 16:R838, 17:R832, 17:R834, 17:R838, 18:R834, 18:R832, 18:R838, 19:R834, 19:R832, 19:R838, 20:R834, 20:R832, 20:R838, 1:R838, 1:R832, 1:R834, 2:R838, 2:R832, 2:R834, 3:R838, 3:R832, 3:R834, 4:R838, 4:R832, 4:R834, 5:R838, 5:R834, 5:R832, 6:R838, 6:R834, 6:R832, 7:R838, 7:R834, 7:R832, 8:R838, 8:R834, 8:R832, 9:R838, 9:R834, 9:R832, 10:R838, 10:R834, 10:R832,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 25    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S9102K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S9102K11-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R841, 9:R841, 8:R841, 7:R841, 6:R841, 5:R841, 4:R841, 3:R841, 2:R841, 1:R841, 20:R841, 19:R841, 18:R841, 17:R841, 16:R841, 15:R841, 14:R841, 13:R841, 12:R841, 11:R841, 30:R841, 29:R841, 28:R841, 27:R841, 26:R841, 25:R841, 24:R841, 23:R841, 22:R841, 21:R841,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 27    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">27   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>02S1030591-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30302S1030591-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:C815, 9:C815, 8:C815, 7:C815, 6:C815, 5:C815, 4:C815, 3:C815, 2:C815, 1:C815, 20:C815, 19:C815, 18:C815, 17:C815, 16:C815, 15:C815, 14:C815, 13:C815, 12:C815, 11:C815, 30:C815, 29:C815, 28:C815, 27:C815, 26:C815, 25:C815, 24:C815, 23:C815, 22:C815, 21:C815,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 28    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">28   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>05S5248100-18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30305S5248100-18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:ZD802, 9:ZD802, 8:ZD802, 7:ZD802, 6:ZD802, 5:ZD802, 4:ZD802, 3:ZD802, 2:ZD802, 1:ZD802, 20:ZD802, 19:ZD802, 18:ZD802, 17:ZD802, 16:ZD802, 15:ZD802, 14:ZD802, 13:ZD802, 12:ZD802, 11:ZD802, 30:ZD802, 29:ZD802, 28:ZD802, 27:ZD802, 26:ZD802, 25:ZD802, 24:ZD802, 23:ZD802, 22:ZD802, 21:ZD802,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 29    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">29   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S0000220-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S0000220-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R828, 9:R828, 8:R828, 7:R828, 6:R828, 5:R828, 4:R828, 3:R828, 2:R828, 1:R828, 20:R828, 19:R828, 18:R828, 17:R828, 16:R828, 15:R828, 14:R828, 13:R828, 12:R828, 11:R828, 30:R828, 29:R828, 28:R828, 27:R828, 26:R828, 25:R828, 24:R828, 23:R828, 22:R828, 21:R828,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 30    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S3302310-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S3302310-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R843, 9:R843, 8:R843, 7:R843, 6:R843, 5:R843, 4:R843, 3:R843, 2:R843, 1:R843, 20:R843, 19:R843, 18:R843, 17:R843, 16:R843, 15:R843, 14:R843, 13:R843, 12:R843, 11:R843, 30:R843, 29:R843, 28:R843, 27:R843, 26:R843, 25:R843, 24:R843, 23:R843, 22:R843, 21:R843,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 31    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">31   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>01S2701210-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30301S2701210-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:R835, 9:R835, 8:R835, 7:R835, 6:R835, 5:R835, 4:R835, 3:R835, 2:R835, 1:R835, 20:R835, 19:R835, 18:R835, 17:R835, 16:R835, 15:R835, 14:R835, 13:R835, 12:R835, 11:R835, 30:R835, 29:R835, 28:R835, 27:R835, 26:R835, 25:R835, 24:R835, 23:R835, 22:R835, 21:R835,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2- 32    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">32   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>05S5242100-18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30305S5242100-18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:ZD800, 9:ZD800, 8:ZD800, 7:ZD800, 6:ZD800, 5:ZD800, 4:ZD800, 3:ZD800, 2:ZD800, 1:ZD800, 20:ZD800, 19:ZD800, 18:ZD800, 17:ZD800, 16:ZD800, 15:ZD800, 14:ZD800, 13:ZD800, 12:ZD800, 11:ZD800, 30:ZD800, 29:ZD800, 28:ZD800, 27:ZD800, 26:ZD800, 25:ZD800, 24:ZD800, 23:ZD800, 22:ZD800, 21:ZD800,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 17    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">17   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>02S4740230-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30302S4740230-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:C806, 9:C806, 8:C806, 7:C806, 6:C806, 5:C806, 4:C806, 3:C806, 2:C806, 1:C806, 20:C806, 19:C806, 18:C806, 17:C806, 16:C806, 15:C806, 14:C806, 13:C806, 12:C806, 11:C806, 30:C806, 29:C806, 28:C806, 27:C806, 26:C806, 25:C806, 24:C806, 23:C806, 22:C806, 21:C806,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 20    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>05S1600000-06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30305S1600000-06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24:D807, 24:D808, 24:D809, 24:D812, 24:D802, 24:D801, 17:D807, 17:D808, 17:D809, 23:D812, 23:D802, 23:D801, 18:D809, 18:D808, 18:D807, 22:D801, 22:D802, 22:D812, 23:D809, 23:D808, 23:D807, 22:D809, 22:D808, 22:D807, 21:D807, 21:D808, 21:D809, 21:D812, 21:D802, 21:D801, 20:D807, 20:D808, 20:D809, 19:D807, 19:D808, 19:D809, 20:D812, 20:D802, 20:D801, 1:D807, 1:D808, 1:D809, 2:D807, 2:D808, 2:D809, 1:D812, 1:D802, 1:D801, 2:D802, 2:D801, 2:D812, 3:D809, 3:D812, 3:D802, 3:D801, 4:D812, 4:D802, 4:D801, 5:D812, 5:D802, 5:D801, 6:D802, 6:D801, 6:D812, 7:D809, 7:D802, 7:D801, 7:D812, 8:D809, 8:D808, 8:D807, 14:D802, 14:D801, 14:D812, 13:D809, 13:D808, 13:D807, 27:D801, 27:D802, 27:D812, 28:D812, 28:D802, 28:D801, 29:D812, 29:D802, 29:D801, 12:D807, 12:D808, 12:D809, 13:D812, 13:D802, 13:D801, 9:D807, 9:D808, 9:D809, 8:D812, 8:D802, 8:D801, 9:D802, 9:D801, 9:D812, 10:D802, 10:D801, 10:D812, 10:D809, 10:D808, 10:D807, 12:D801, 12:D802, 12:D812, 11:D802, 11:D801, 11:D812, 11:D809, 11:D808, 11:D807, 30:D801, 30:D802, 30:D812, 30:D809, 30:D808, 30:D807, 29:D809, 29:D808, 29:D807, 28:D809, 28:D808, 28:D807, 27:D807, 27:D808, 27:D809, 26:D812, 26:D802, 26:D801, 14:D807, 14:D808, 14:D809, 15:D807, 15:D808, 15:D809, 15:D812, 15:D802, 15:D801, 7:D807, 7:D808, 6:D809, 6:D808, 6:D807, 16:D801, 16:D802, 16:D812, 5:D807, 5:D808, 5:D809, 4:D809, 3:D808, 3:D807, 19:D802, 19:D801, 19:D812, 18:D812, 18:D802, 18:D801, 4:D808, 4:D807, 17:D801, 17:D802, 17:D812, 16:D809, 16:D808, 16:D807, 25:D802, 25:D801, 25:D812, 26:D809, 26:D808, 26:D807, 25:D809, 25:D808, 25:D807,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 22    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>06S2222001-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30306S2222001-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:Q808, 10:Q809, 9:Q808, 9:Q809, 8:Q808, 8:Q809, 7:Q808, 7:Q809, 6:Q808, 6:Q809, 5:Q808, 5:Q809, 4:Q808, 4:Q809, 3:Q808, 3:Q809, 2:Q808, 2:Q809, 1:Q808, 1:Q809, 20:Q809, 20:Q808, 19:Q809, 19:Q808, 18:Q809, 18:Q808, 17:Q809, 17:Q808, 16:Q809, 16:Q808, 15:Q809, 15:Q808, 14:Q809, 14:Q808, 13:Q809, 13:Q808, 12:Q809, 12:Q808, 11:Q809, 11:Q808, 30:Q808, 30:Q809, 29:Q808, 29:Q809, 28:Q808, 28:Q809, 27:Q808, 27:Q809, 26:Q808, 26:Q809, 25:Q808, 25:Q809, 24:Q808, 24:Q809, 23:Q808, 23:Q809, 22:Q808, 22:Q809, 21:Q808, 21:Q809,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 23    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>02S1040530-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30302S1040530-00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:C811, 9:C811, 8:C811, 7:C811, 6:C811, 5:C811, 4:C811, 3:C811, 2:C811, 1:C811, 20:C811, 19:C811, 18:C811, 17:C811, 16:C811, 15:C811, 14:C811, 13:C811, 12:C811, 11:C811, 30:C811, 29:C811, 28:C811, 27:C811, 26:C811, 25:C811, 24:C811, 23:C811, 22:C811, 21:C811,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 24    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>06S2907001-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30306S2907001-24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:Q810, 9:Q810, 8:Q810, 7:Q810, 6:Q810, 5:Q810, 4:Q810, 3:Q810, 2:Q810, 1:Q810, 20:Q810, 19:Q810, 18:Q810, 17:Q810, 16:Q810, 15:Q810, 14:Q810, 13:Q810, 12:Q810, 11:Q810, 30:Q810, 29:Q810, 28:Q810, 27:Q810, 26:Q810, 25:Q810, 24:Q810, 23:Q810, 22:Q810, 21:Q810,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 28    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>04S2206201-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30304S2206201-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:TVS800, 9:TVS800, 8:TVS800, 7:TVS800, 6:TVS800, 5:TVS800, 4:TVS800, 3:TVS800, 2:TVS800, 1:TVS800, 20:TVS800, 19:TVS800, 18:TVS800, 17:TVS800, 16:TVS800, 15:TVS800, 14:TVS800, 13:TVS800, 12:TVS800, 11:TVS800, 30:TVS800, 29:TVS800, 28:TVS800, 27:TVS800, 26:TVS800, 25:TVS800, 24:TVS800, 23:TVS800, 22:TVS800, 21:TVS800,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KT-1200F-180</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3- 30    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>07S5190001-50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30307S5190001-50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30:U802, 29:U802, 28:U802, 27:U802, 26:U802, 25:U802, 24:U802, 23:U802, 22:U802, 21:U802, 20:U802, 19:U802, 18:U802, 17:U802, 16:U802, 15:U802, 14:U802, 13:U802, 12:U802, 11:U802, 10:U802, 9:U802, 8:U802, 7:U802, 6:U802, 5:U802, 4:U802, 3:U802, 2:U802, 1:U802,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KT-1600F-380</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4- 11    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">11   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>05S2100001-06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30305S2100001-06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:D811, 9:D811, 8:D811, 7:D811, 6:D811, 5:D811, 4:D811, 3:D811, 2:D811, 1:D811, 20:D811, 19:D811, 18:D811, 17:D811, 16:D811, 15:D811, 14:D811, 13:D811, 12:D811, 11:D811, 30:D811, 29:D811, 28:D811, 27:D811, 26:D811, 25:D811, 24:D811, 23:D811, 22:D811, 21:D811,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4- 14    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>05SGU1M000-03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30305SGU1M000-03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:D806, 10:D805, 9:D806, 9:D805, 8:D806, 8:D805, 7:D806, 7:D805, 6:D806, 6:D805, 5:D806, 5:D805, 4:D806, 4:D805, 3:D806, 3:D805, 2:D806, 2:D805, 1:D806, 1:D805, 20:D805, 20:D806, 19:D805, 19:D806, 18:D805, 18:D806, 17:D805, 17:D806, 16:D805, 16:D806, 15:D805, 15:D806, 14:D805, 14:D806, 13:D805, 13:D806, 12:D805, 12:D806, 11:D805, 11:D806, 30:D806, 30:D805, 29:D806, 29:D805, 28:D806, 28:D805, 27:D806, 27:D805, 26:D806, 26:D805, 25:D806, 25:D805, 24:D806, 24:D805, 23:D806, 23:D805, 22:D806, 22:D805, 21:D806, 21:D805,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4- 23    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>07C8170003-10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30307C8170003-10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:U800, 10:U803, 9:U800, 9:U803, 8:U800, 8:U803, 7:U800, 7:U803, 6:U800, 6:U803, 5:U800, 5:U803, 4:U800, 4:U803, 3:U800, 3:U803, 2:U800, 2:U803, 1:U800, 1:U803, 20:U803, 20:U800, 19:U803, 19:U800, 18:U803, 18:U800, 17:U803, 17:U800, 16:U803, 16:U800, 15:U803, 15:U800, 14:U803, 14:U800, 13:U803, 13:U800, 12:U803, 12:U800, 11:U803, 11:U800, 30:U800, 30:U803, 29:U800, 29:U803, 28:U800, 28:U803, 27:U800, 27:U803, 26:U800, 26:U803, 25:U800, 25:U803, 24:U800, 24:U803, 23:U800, 23:U803, 22:U800, 22:U803, 21:U800, 21:U803,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4- 30    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>04S2516101-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30304S2516101-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:TVS801, 9:TVS801, 8:TVS801, 7:TVS801, 6:TVS801, 5:TVS801, 4:TVS801, 3:TVS801, 2:TVS801, 1:TVS801, 20:TVS801, 19:TVS801, 18:TVS801, 17:TVS801, 16:TVS801, 15:TVS801, 14:TVS801, 13:TVS801, 12:TVS801, 11:TVS801, 30:TVS801, 29:TVS801, 28:TVS801, 27:TVS801, 26:TVS801, 25:TVS801, 24:TVS801, 23:TVS801, 22:TVS801, 21:TVS801,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4- 36    </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">36   </x:t>
+  </x:si>
+  <x:si>
+    <x:t>07S7600301-50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MX2CDCCAQ600C00-F30307S7600301-50</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30:U805, 29:U805, 28:U805, 27:U805, 26:U805, 25:U805, 24:U805, 23:U805, 22:U805, 21:U805, 20:U805, 19:U805, 18:U805, 17:U805, 16:U805, 15:U805, 14:U805, 13:U805, 12:U805, 11:U805, 10:U805, 9:U805, 8:U805, 7:U805, 6:U805, 5:U805, 4:U805, 3:U805, 2:U805, 1:U805,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">4- 8     </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">8    </x:t>
+  </x:si>
+  <x:si>
     <x:t>13J0000058-00</x:t>
   </x:si>
   <x:si>
@@ -116,21 +578,12 @@
     <x:t>MX2CDCCAQ600C00-F30301S5101310-00</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">30   </x:t>
-  </x:si>
-  <x:si>
     <x:t>1:R826, 2:R826, 3:R826, 4:R826, 5:R826, 6:R826, 7:R826, 8:R826, 9:R826, 10:R826, 20:R826, 19:R826, 18:R826, 17:R826, 16:R826, 15:R826, 14:R826, 13:R826, 12:R826, 11:R826, 21:R826, 22:R826, 23:R826, 24:R826, 25:R826, 26:R826, 27:R826, 28:R826, 29:R826, 30:R826,</x:t>
   </x:si>
   <x:si>
-    <x:t>KT-0800F-180</x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">1- 16    </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">1    </x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">16   </x:t>
   </x:si>
   <x:si>
@@ -152,69 +605,15 @@
     <x:t xml:space="preserve">18   </x:t>
   </x:si>
   <x:si>
-    <x:t>01S1001K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S1001K11-00</x:t>
-  </x:si>
-  <x:si>
     <x:t>10:R852, 9:R852, 8:R852, 7:R852, 6:R852, 5:R852, 4:R852, 3:R852, 2:R852, 1:R852, 20:R852, 19:R852, 18:R852, 17:R852, 16:R852, 15:R852, 14:R852, 13:R852, 12:R852, 11:R852, 30:R852, 29:R852, 28:R852, 27:R852, 26:R852, 25:R852, 24:R852, 23:R852, 22:R852, 21:R852,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">1- 20    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">20   </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">150  </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R811, 9:R811, 8:R811, 7:R811, 6:R811, 5:R811, 4:R811, 3:R811, 2:R811, 1:R811, 10:R809, 9:R809, 8:R809, 7:R809, 6:R809, 5:R809, 4:R809, 3:R809, 2:R809, 1:R809, 10:R806, 9:R806, 8:R806, 7:R806, 6:R806, 5:R806, 4:R806, 3:R806, 2:R806, 1:R806, 10:R844, 9:R844, 8:R844, 7:R844, 6:R844, 5:R844, 4:R844, 3:R844, 2:R844, 1:R844, 10:R849, 9:R849, 8:R849, 7:R849, 6:R849, 5:R849, 4:R849, 3:R849, 2:R849, 1:R849, 11:R811, 12:R811, 13:R811, 14:R811, 15:R811, 16:R811, 17:R811, 18:R811, 19:R811, 20:R811, 11:R809, 12:R809, 13:R809, 14:R809, 15:R809, 16:R809, 17:R809, 18:R809, 19:R809, 20:R809, 11:R806, 12:R806, 13:R806, 14:R806, 15:R806, 16:R806, 17:R806, 18:R806, 19:R806, 20:R806, 11:R844, 12:R844, 13:R844, 14:R844, 15:R844, 16:R844, 17:R844, 18:R844, 19:R844, 20:R844, 11:R849, 12:R849, 13:R849, 14:R849, 15:R849, 16:R849, 17:R849, 18:R849, 19:R849, 20:R849, 30:R811, 29:R811, 28:R811, 27:R811, 26:R811, 25:R811, 24:R811, 23:R811, 22:R811, 21:R811, 30:R809, 29:R809, 28:R809, 27:R809, 26:R809, 25:R809, 24:R809, 23:R809, 22:R809, 21:R809, 30:R806, 29:R806, 28:R806, 27:R806, 26:R806, 25:R806, 24:R806, 23:R806, 22:R806, 21:R806, 30:R844, 29:R844, 28:R844, 27:R844, 26:R844, 25:R844, 24:R844, 23:R844, 22:R844, 21:R844, 30:R849, 29:R849, 28:R849, 27:R849, 26:R849, 25:R849, 24:R849, 23:R849, 22:R849, 21:R849,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bottom</x:t>
-  </x:si>
-  <x:si>
-    <x:t>02S1050001-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30302S1050001-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">60   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:C807, 9:C807, 8:C807, 7:C807, 6:C807, 5:C807, 4:C807, 3:C807, 2:C807, 1:C807, 10:C808, 9:C808, 8:C808, 7:C808, 6:C808, 5:C808, 4:C808, 3:C808, 2:C808, 1:C808, 11:C807, 12:C807, 13:C807, 14:C807, 15:C807, 16:C807, 17:C807, 18:C807, 19:C807, 20:C807, 11:C808, 12:C808, 13:C808, 14:C808, 15:C808, 16:C808, 17:C808, 18:C808, 19:C808, 20:C808, 30:C807, 29:C807, 28:C807, 27:C807, 26:C807, 25:C807, 24:C807, 23:C807, 22:C807, 21:C807, 30:C808, 29:C808, 28:C808, 27:C808, 26:C808, 25:C808, 24:C808, 23:C808, 22:C808, 21:C808,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">1- 21    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">21   </x:t>
-  </x:si>
-  <x:si>
     <x:t>10:C816, 9:C816, 8:C816, 7:C816, 6:C816, 5:C816, 4:C816, 3:C816, 2:C816, 1:C816, 20:C816, 19:C816, 18:C816, 17:C816, 16:C816, 15:C816, 14:C816, 13:C816, 12:C816, 11:C816, 30:C816, 29:C816, 28:C816, 27:C816, 26:C816, 25:C816, 24:C816, 23:C816, 22:C816, 21:C816,</x:t>
   </x:si>
   <x:si>
-    <x:t>01S3302K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S3302K11-00</x:t>
-  </x:si>
-  <x:si>
     <x:t>10:R802, 9:R802, 8:R802, 7:R802, 6:R802, 5:R802, 4:R802, 3:R802, 2:R802, 1:R802, 20:R802, 19:R802, 18:R802, 17:R802, 16:R802, 15:R802, 14:R802, 13:R802, 12:R802, 11:R802, 30:R802, 29:R802, 28:R802, 27:R802, 26:R802, 25:R802, 24:R802, 23:R802, 22:R802, 21:R802,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">1- 22    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">22   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R818, 9:R818, 8:R818, 7:R818, 6:R818, 5:R818, 4:R818, 3:R818, 2:R818, 1:R818, 11:R818, 12:R818, 13:R818, 14:R818, 15:R818, 16:R818, 17:R818, 18:R818, 19:R818, 20:R818, 30:R818, 29:R818, 28:R818, 27:R818, 26:R818, 25:R818, 24:R818, 23:R818, 22:R818, 21:R818,</x:t>
-  </x:si>
-  <x:si>
     <x:t>01S5600K11-00</x:t>
   </x:si>
   <x:si>
@@ -227,63 +626,12 @@
     <x:t xml:space="preserve">1- 23    </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">23   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S6800K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S6800K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R815, 9:R815, 8:R815, 7:R815, 6:R815, 5:R815, 4:R815, 3:R815, 2:R815, 1:R815, 10:R824, 9:R824, 8:R824, 7:R824, 6:R824, 5:R824, 4:R824, 3:R824, 2:R824, 1:R824, 11:R815, 12:R815, 13:R815, 14:R815, 15:R815, 16:R815, 17:R815, 18:R815, 19:R815, 20:R815, 11:R824, 12:R824, 13:R824, 14:R824, 15:R824, 16:R824, 17:R824, 18:R824, 19:R824, 20:R824, 30:R815, 29:R815, 28:R815, 27:R815, 26:R815, 25:R815, 24:R815, 23:R815, 22:R815, 21:R815, 30:R824, 29:R824, 28:R824, 26:R824, 27:R824, 25:R824, 24:R824, 23:R824, 22:R824, 21:R824,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">1- 24    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">24   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S1003K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S1003K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">90   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R842, 9:R842, 8:R842, 7:R842, 6:R842, 5:R842, 4:R842, 3:R842, 2:R842, 1:R842, 10:R839, 9:R839, 8:R839, 7:R839, 6:R839, 5:R839, 4:R839, 3:R839, 2:R839, 1:R839, 10:R836, 9:R836, 8:R836, 7:R836, 6:R836, 5:R836, 4:R836, 3:R836, 2:R836, 1:R836, 11:R842, 12:R842, 13:R842, 14:R842, 15:R842, 16:R842, 17:R842, 18:R842, 19:R842, 20:R842, 11:R839, 12:R839, 13:R839, 14:R839, 15:R839, 16:R839, 17:R839, 18:R839, 19:R839, 20:R839, 11:R836, 12:R836, 13:R836, 14:R836, 15:R836, 16:R836, 17:R836, 18:R836, 19:R836, 20:R836, 30:R842, 29:R842, 28:R842, 27:R842, 26:R842, 25:R842, 24:R842, 23:R842, 22:R842, 21:R842, 30:R839, 29:R839, 28:R839, 27:R839, 26:R839, 25:R839, 24:R839, 23:R839, 22:R839, 21:R839, 30:R836, 29:R836, 28:R836, 27:R836, 26:R836, 25:R836, 24:R836, 23:R836, 22:R836, 21:R836,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">1- 25    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">25   </x:t>
-  </x:si>
-  <x:si>
     <x:t>10:R823, 9:R823, 8:R823, 7:R823, 6:R823, 5:R823, 4:R823, 3:R823, 2:R823, 1:R823, 10:R814, 9:R814, 8:R814, 7:R814, 6:R814, 5:R814, 4:R814, 3:R814, 2:R814, 1:R814, 20:R823, 19:R823, 18:R823, 17:R823, 16:R823, 15:R823, 14:R823, 13:R823, 12:R823, 11:R823, 20:R814, 19:R814, 18:R814, 17:R814, 16:R814, 15:R814, 14:R814, 13:R814, 12:R814, 11:R814, 30:R823, 29:R823, 28:R823, 27:R823, 26:R823, 25:R823, 24:R823, 23:R823, 22:R823, 21:R823, 30:R814, 29:R814, 28:R814, 27:R814, 26:R814, 25:R814, 24:R814, 23:R814, 22:R814, 21:R814,</x:t>
   </x:si>
   <x:si>
-    <x:t>01S5101K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S5101K11-00</x:t>
-  </x:si>
-  <x:si>
     <x:t>10:R827, 9:R827, 8:R827, 7:R827, 6:R827, 5:R827, 4:R827, 3:R827, 2:R827, 1:R827, 10:R848, 9:R848, 8:R848, 7:R848, 6:R848, 5:R848, 4:R848, 3:R848, 2:R848, 1:R848, 10:R850, 9:R850, 8:R850, 7:R850, 6:R850, 5:R850, 4:R850, 3:R850, 2:R850, 1:R850, 10:R801, 9:R801, 8:R801, 7:R801, 6:R801, 5:R801, 4:R801, 3:R801, 2:R801, 1:R801, 20:R827, 19:R827, 18:R827, 17:R827, 16:R827, 15:R827, 14:R827, 13:R827, 12:R827, 11:R827, 20:R848, 19:R848, 18:R848, 17:R848, 16:R848, 15:R848, 14:R848, 13:R848, 12:R848, 11:R848, 20:R850, 19:R850, 18:R850, 17:R850, 16:R850, 15:R850, 14:R850, 13:R850, 12:R850, 11:R850, 20:R801, 19:R801, 18:R801, 17:R801, 16:R801, 15:R801, 14:R801, 13:R801, 12:R801, 11:R801, 30:R827, 29:R827, 28:R827, 27:R827, 26:R827, 25:R827, 24:R827, 23:R827, 22:R827, 21:R827, 30:R848, 29:R848, 28:R848, 27:R848, 26:R848, 25:R848, 24:R848, 23:R848, 22:R848, 21:R848, 30:R850, 29:R850, 28:R850, 27:R850, 26:R850, 25:R850, 24:R850, 23:R850, 22:R850, 21:R850, 30:R801, 29:R801, 28:R801, 27:R801, 26:R801, 25:R801, 24:R801, 23:R801, 22:R801, 21:R801,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">1- 26    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">26   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R820, 10:R822, 9:R820, 9:R822, 8:R820, 8:R822, 7:R820, 7:R822, 6:R820, 6:R822, 5:R820, 5:R822, 4:R820, 4:R822, 3:R820, 3:R822, 2:R820, 2:R822, 1:R820, 1:R822, 11:R820, 11:R822, 12:R820, 12:R822, 13:R820, 13:R822, 14:R820, 14:R822, 15:R820, 15:R822, 16:R820, 16:R822, 17:R820, 17:R822, 18:R820, 18:R822, 19:R820, 19:R822, 20:R820, 20:R822, 30:R820, 30:R822, 29:R820, 29:R822, 28:R820, 28:R822, 27:R820, 27:R822, 26:R820, 26:R822, 25:R820, 25:R822, 24:R820, 24:R822, 23:R820, 23:R822, 22:R820, 22:R822, 21:R820, 21:R822,</x:t>
-  </x:si>
-  <x:si>
     <x:t>01S3901K11-00</x:t>
   </x:si>
   <x:si>
@@ -296,9 +644,6 @@
     <x:t xml:space="preserve">1- 27    </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">27   </x:t>
-  </x:si>
-  <x:si>
     <x:t>01S1602K11-00</x:t>
   </x:si>
   <x:si>
@@ -311,9 +656,6 @@
     <x:t xml:space="preserve">1- 28    </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">28   </x:t>
-  </x:si>
-  <x:si>
     <x:t>01S2203310-00</x:t>
   </x:si>
   <x:si>
@@ -326,27 +668,9 @@
     <x:t xml:space="preserve">2- 13    </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">2    </x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">13   </x:t>
   </x:si>
   <x:si>
-    <x:t>01S1002310-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S1002310-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R833, 9:R833, 8:R833, 7:R833, 6:R833, 5:R833, 4:R833, 3:R833, 2:R833, 1:R833, 20:R833, 19:R833, 18:R833, 17:R833, 16:R833, 15:R833, 14:R833, 13:R833, 12:R833, 11:R833, 30:R833, 29:R833, 28:R833, 27:R833, 26:R833, 25:R833, 24:R833, 23:R833, 22:R833, 21:R833,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 14    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">14   </x:t>
-  </x:si>
-  <x:si>
     <x:t>01S6201310-00</x:t>
   </x:si>
   <x:si>
@@ -374,162 +698,18 @@
     <x:t xml:space="preserve">19   </x:t>
   </x:si>
   <x:si>
-    <x:t>01S5102K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S5102K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R805, 9:R805, 8:R805, 7:R805, 6:R805, 5:R805, 4:R805, 3:R805, 2:R805, 1:R805, 20:R805, 19:R805, 18:R805, 17:R805, 16:R805, 15:R805, 14:R805, 13:R805, 12:R805, 11:R805, 30:R805, 29:R805, 28:R805, 27:R805, 26:R805, 25:R805, 24:R805, 23:R805, 22:R805, 21:R805,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 20    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S1002K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S1002K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R846, 9:R846, 8:R846, 7:R846, 6:R846, 5:R846, 4:R846, 3:R846, 2:R846, 1:R846, 20:R846, 19:R846, 18:R846, 17:R846, 16:R846, 15:R846, 14:R846, 13:R846, 12:R846, 11:R846, 30:R846, 29:R846, 28:R846, 27:R846, 26:R846, 25:R846, 24:R846, 23:R846, 22:R846, 21:R846,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 22    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">180  </x:t>
-  </x:si>
-  <x:si>
     <x:t>1:R819, 1:R808, 1:R825, 1:R821, 2:R808, 2:R825, 2:R821, 2:R819, 3:R808, 3:R825, 3:R821, 3:R819, 4:R808, 4:R825, 4:R821, 4:R819, 5:R808, 5:R825, 5:R821, 5:R819, 6:R808, 6:R825, 6:R821, 6:R819, 7:R808, 7:R825, 7:R821, 7:R819, 8:R808, 8:R825, 8:R821, 8:R819, 9:R808, 9:R825, 9:R821, 9:R819, 10:R819, 10:R808, 10:R825, 10:R821, 10:R816, 10:R807, 20:R819, 20:R821, 20:R825, 20:R808, 9:R816, 9:R807, 19:R819, 19:R821, 19:R825, 19:R808, 8:R816, 8:R807, 18:R819, 18:R821, 18:R825, 18:R808, 7:R816, 7:R807, 17:R819, 17:R821, 17:R825, 17:R808, 6:R816, 6:R807, 16:R819, 16:R821, 16:R825, 16:R808, 5:R816, 5:R807, 15:R819, 15:R821, 15:R825, 15:R808, 4:R816, 4:R807, 14:R819, 14:R821, 14:R825, 14:R808, 3:R816, 3:R807, 13:R819, 13:R821, 13:R825, 13:R808, 2:R816, 2:R807, 12:R819, 12:R821, 12:R825, 12:R808, 1:R816, 1:R807, 11:R819, 11:R808, 11:R825, 11:R821, 11:R816, 11:R807, 21:R819, 21:R808, 21:R825, 21:R821, 22:R808, 22:R825, 22:R821, 22:R819, 12:R807, 12:R816, 23:R808, 23:R825, 23:R821, 23:R819, 13:R807, 13:R816, 24:R808, 24:R825, 24:R821, 24:R819, 14:R807, 14:R816, 25:R808, 25:R825, 25:R821, 25:R819, 15:R807, 15:R816, 26:R808, 26:R825, 26:R821, 26:R819, 16:R807, 16:R816, 27:R808, 27:R825, 27:R821, 27:R819, 17:R807, 17:R816, 28:R808, 28:R825, 28:R821, 28:R819, 18:R807, 18:R816, 29:R808, 29:R825, 29:R821, 29:R819, 19:R807, 19:R816, 20:R816, 20:R807, 30:R819, 30:R808, 30:R825, 30:R821, 30:R816, 30:R807, 29:R816, 29:R807, 28:R816, 28:R807, 27:R816, 27:R807, 26:R816, 26:R807, 25:R816, 25:R807, 24:R816, 24:R807, 23:R816, 23:R807, 22:R816, 22:R807, 21:R816, 21:R807,</x:t>
   </x:si>
   <x:si>
-    <x:t>02S1040201-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30302S1040201-00</x:t>
-  </x:si>
-  <x:si>
     <x:t>3:C819, 4:C819, 5:C819, 6:C819, 7:C819, 8:C819, 9:C819, 10:C819, 10:C814, 20:C819, 9:C814, 19:C819, 8:C814, 18:C819, 7:C814, 17:C819, 6:C814, 16:C819, 5:C814, 15:C819, 4:C814, 14:C819, 3:C814, 13:C819, 2:C814, 2:C819, 1:C819, 1:C814, 12:C819, 11:C819, 11:C814, 22:C819, 12:C814, 23:C819, 13:C814, 24:C819, 14:C814, 25:C819, 15:C814, 26:C819, 16:C814, 27:C819, 17:C814, 28:C819, 18:C814, 29:C819, 19:C814, 20:C814, 30:C819, 30:C814, 29:C814, 28:C814, 27:C814, 26:C814, 25:C814, 24:C814, 23:C814, 22:C814, 21:C814, 21:C819,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">2- 23    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>20:C813, 20:C817, 21:C804, 21:C805, 21:C803, 21:C818, 21:C813, 21:C817, 22:C817, 22:C813, 22:C818, 22:C803, 22:C805, 22:C804, 19:C817, 19:C813, 18:C813, 18:C817, 24:C804, 24:C805, 24:C803, 24:C818, 23:C804, 23:C805, 23:C803, 23:C818, 23:C813, 23:C817, 24:C813, 24:C817, 25:C817, 25:C813, 25:C818, 25:C803, 25:C805, 25:C804, 16:C817, 16:C813, 17:C817, 17:C813, 17:C818, 17:C803, 17:C805, 17:C804, 16:C818, 16:C803, 16:C805, 16:C804, 4:C817, 4:C813, 3:C813, 3:C817, 18:C804, 18:C805, 18:C803, 18:C818, 19:C804, 19:C805, 19:C803, 19:C818, 20:C803, 20:C805, 20:C818, 20:C804, 1:C817, 1:C813, 1:C818, 1:C803, 1:C805, 1:C804, 2:C804, 2:C805, 2:C803, 2:C818, 2:C813, 2:C817, 3:C818, 3:C803, 3:C805, 3:C804, 4:C818, 4:C803, 4:C805, 4:C804, 5:C804, 5:C805, 5:C803, 5:C818, 5:C813, 5:C817, 6:C803, 6:C805, 6:C804, 6:C818, 6:C813, 6:C817, 7:C817, 7:C813, 7:C818, 7:C803, 7:C805, 7:C804, 8:C818, 8:C804, 8:C805, 8:C803, 8:C813, 8:C817, 9:C818, 9:C803, 9:C805, 9:C804, 10:C804, 10:C805, 10:C803, 10:C818, 10:C813, 10:C817, 9:C813, 9:C817, 11:C804, 11:C805, 11:C803, 11:C818, 12:C804, 12:C805, 12:C803, 12:C818, 13:C817, 13:C813, 13:C818, 13:C803, 13:C805, 13:C804, 14:C804, 14:C805, 14:C803, 14:C818, 15:C804, 15:C805, 15:C803, 15:C818, 15:C813, 15:C817, 26:C804, 26:C805, 26:C803, 26:C818, 26:C813, 26:C817, 27:C817, 27:C813, 27:C818, 27:C803, 27:C805, 27:C804, 14:C817, 14:C813, 28:C803, 28:C805, 28:C818, 28:C804, 29:C818, 29:C803, 29:C805, 29:C804, 12:C817, 12:C813, 11:C813, 11:C817, 30:C804, 30:C805, 30:C803, 30:C818, 30:C813, 30:C817, 29:C817, 29:C813, 28:C817, 28:C813,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S2001K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S2001K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23:R840, 24:R840, 25:R840, 26:R840, 27:R840, 28:R840, 29:R840, 30:R840, 30:R812, 30:R813, 11:R840, 11:R812, 11:R813, 12:R812, 12:R813, 13:R812, 13:R813, 12:R840, 29:R812, 29:R813, 28:R812, 28:R813, 13:R840, 27:R812, 27:R813, 14:R840, 14:R812, 14:R813, 15:R812, 15:R813, 16:R812, 16:R813, 15:R840, 26:R812, 26:R813, 25:R812, 25:R813, 16:R840, 24:R812, 24:R813, 23:R812, 23:R813, 22:R812, 22:R813, 18:R840, 17:R840, 17:R812, 17:R813, 18:R812, 18:R813, 19:R812, 19:R813, 3:R840, 4:R840, 5:R840, 6:R840, 7:R840, 8:R840, 9:R840, 10:R840, 10:R812, 10:R813, 9:R812, 9:R813, 8:R812, 8:R813, 7:R812, 7:R813, 6:R812, 6:R813, 5:R812, 5:R813, 4:R812, 4:R813, 3:R812, 3:R813, 2:R812, 2:R813, 1:R812, 1:R813, 2:R840, 1:R840, 20:R812, 20:R813, 19:R840, 20:R840, 21:R812, 21:R813, 22:R840, 21:R840,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 24    </x:t>
-  </x:si>
-  <x:si>
     <x:t>30:R859, 30:R861, 29:R859, 29:R861, 28:R859, 28:R861, 27:R859, 27:R861, 26:R859, 26:R861, 25:R859, 25:R861, 24:R859, 24:R861, 23:R859, 23:R861, 22:R859, 22:R861, 21:R859, 21:R861, 11:R861, 11:R859, 12:R861, 12:R859, 13:R861, 13:R859, 14:R861, 14:R859, 15:R861, 15:R859, 16:R861, 16:R859, 17:R861, 17:R859, 18:R861, 18:R859, 19:R861, 19:R859, 20:R861, 20:R859, 10:R859, 10:R861, 9:R859, 9:R861, 8:R859, 8:R861, 7:R859, 7:R861, 6:R859, 6:R861, 5:R859, 5:R861, 4:R859, 4:R861, 3:R859, 3:R861, 2:R859, 2:R861, 1:R859, 1:R861,</x:t>
   </x:si>
   <x:si>
-    <x:t>01S2002K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S2002K11-00</x:t>
-  </x:si>
-  <x:si>
     <x:t>30:R858, 30:R845, 29:R858, 29:R845, 28:R858, 28:R845, 27:R858, 27:R845, 26:R858, 26:R845, 25:R858, 25:R845, 24:R858, 24:R845, 23:R858, 23:R845, 22:R858, 22:R845, 21:R858, 21:R845, 11:R845, 11:R858, 12:R845, 12:R858, 13:R845, 13:R858, 14:R845, 14:R858, 15:R845, 15:R858, 16:R845, 16:R858, 17:R845, 17:R858, 18:R845, 18:R858, 19:R845, 19:R858, 20:R845, 20:R858, 10:R858, 10:R845, 9:R858, 9:R845, 8:R858, 8:R845, 7:R858, 7:R845, 6:R858, 6:R845, 5:R858, 5:R845, 4:R858, 4:R845, 3:R858, 3:R845, 2:R858, 2:R845, 1:R858, 1:R845,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">2- 25    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>21:R838, 21:R832, 21:R834, 22:R838, 22:R834, 22:R832, 23:R838, 23:R832, 23:R834, 24:R838, 24:R834, 24:R832, 25:R838, 25:R834, 25:R832, 26:R838, 26:R834, 26:R832, 27:R838, 27:R834, 27:R832, 28:R838, 28:R834, 28:R832, 29:R838, 29:R834, 29:R832, 30:R838, 30:R834, 30:R832, 11:R834, 11:R832, 11:R838, 12:R834, 12:R832, 12:R838, 13:R832, 13:R834, 13:R838, 14:R832, 14:R834, 14:R838, 15:R832, 15:R834, 15:R838, 16:R832, 16:R834, 16:R838, 17:R832, 17:R834, 17:R838, 18:R834, 18:R832, 18:R838, 19:R834, 19:R832, 19:R838, 20:R834, 20:R832, 20:R838, 1:R838, 1:R832, 1:R834, 2:R838, 2:R832, 2:R834, 3:R838, 3:R832, 3:R834, 4:R838, 4:R832, 4:R834, 5:R838, 5:R834, 5:R832, 6:R838, 6:R834, 6:R832, 7:R838, 7:R834, 7:R832, 8:R838, 8:R834, 8:R832, 9:R838, 9:R834, 9:R832, 10:R838, 10:R834, 10:R832,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S9102K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S9102K11-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R841, 9:R841, 8:R841, 7:R841, 6:R841, 5:R841, 4:R841, 3:R841, 2:R841, 1:R841, 20:R841, 19:R841, 18:R841, 17:R841, 16:R841, 15:R841, 14:R841, 13:R841, 12:R841, 11:R841, 30:R841, 29:R841, 28:R841, 27:R841, 26:R841, 25:R841, 24:R841, 23:R841, 22:R841, 21:R841,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 27    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>02S1030591-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30302S1030591-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:C815, 9:C815, 8:C815, 7:C815, 6:C815, 5:C815, 4:C815, 3:C815, 2:C815, 1:C815, 20:C815, 19:C815, 18:C815, 17:C815, 16:C815, 15:C815, 14:C815, 13:C815, 12:C815, 11:C815, 30:C815, 29:C815, 28:C815, 27:C815, 26:C815, 25:C815, 24:C815, 23:C815, 22:C815, 21:C815,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 28    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>05S5248100-18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30305S5248100-18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:ZD802, 9:ZD802, 8:ZD802, 7:ZD802, 6:ZD802, 5:ZD802, 4:ZD802, 3:ZD802, 2:ZD802, 1:ZD802, 20:ZD802, 19:ZD802, 18:ZD802, 17:ZD802, 16:ZD802, 15:ZD802, 14:ZD802, 13:ZD802, 12:ZD802, 11:ZD802, 30:ZD802, 29:ZD802, 28:ZD802, 27:ZD802, 26:ZD802, 25:ZD802, 24:ZD802, 23:ZD802, 22:ZD802, 21:ZD802,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 29    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">29   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S0000220-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S0000220-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R828, 9:R828, 8:R828, 7:R828, 6:R828, 5:R828, 4:R828, 3:R828, 2:R828, 1:R828, 20:R828, 19:R828, 18:R828, 17:R828, 16:R828, 15:R828, 14:R828, 13:R828, 12:R828, 11:R828, 30:R828, 29:R828, 28:R828, 27:R828, 26:R828, 25:R828, 24:R828, 23:R828, 22:R828, 21:R828,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 30    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S3302310-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S3302310-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R843, 9:R843, 8:R843, 7:R843, 6:R843, 5:R843, 4:R843, 3:R843, 2:R843, 1:R843, 20:R843, 19:R843, 18:R843, 17:R843, 16:R843, 15:R843, 14:R843, 13:R843, 12:R843, 11:R843, 30:R843, 29:R843, 28:R843, 27:R843, 26:R843, 25:R843, 24:R843, 23:R843, 22:R843, 21:R843,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 31    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">31   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>01S2701210-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30301S2701210-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:R835, 9:R835, 8:R835, 7:R835, 6:R835, 5:R835, 4:R835, 3:R835, 2:R835, 1:R835, 20:R835, 19:R835, 18:R835, 17:R835, 16:R835, 15:R835, 14:R835, 13:R835, 12:R835, 11:R835, 30:R835, 29:R835, 28:R835, 27:R835, 26:R835, 25:R835, 24:R835, 23:R835, 22:R835, 21:R835,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">2- 32    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">32   </x:t>
-  </x:si>
-  <x:si>
     <x:t>01S4301310-00</x:t>
   </x:si>
   <x:si>
@@ -542,78 +722,12 @@
     <x:t xml:space="preserve">3- 16    </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">3    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>05S5242100-18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30305S5242100-18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:ZD800, 9:ZD800, 8:ZD800, 7:ZD800, 6:ZD800, 5:ZD800, 4:ZD800, 3:ZD800, 2:ZD800, 1:ZD800, 20:ZD800, 19:ZD800, 18:ZD800, 17:ZD800, 16:ZD800, 15:ZD800, 14:ZD800, 13:ZD800, 12:ZD800, 11:ZD800, 30:ZD800, 29:ZD800, 28:ZD800, 27:ZD800, 26:ZD800, 25:ZD800, 24:ZD800, 23:ZD800, 22:ZD800, 21:ZD800,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">3- 17    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">17   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>02S4740230-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30302S4740230-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:C806, 9:C806, 8:C806, 7:C806, 6:C806, 5:C806, 4:C806, 3:C806, 2:C806, 1:C806, 20:C806, 19:C806, 18:C806, 17:C806, 16:C806, 15:C806, 14:C806, 13:C806, 12:C806, 11:C806, 30:C806, 29:C806, 28:C806, 27:C806, 26:C806, 25:C806, 24:C806, 23:C806, 22:C806, 21:C806,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">3- 20    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>05S1600000-06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30305S1600000-06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24:D807, 24:D808, 24:D809, 24:D812, 24:D802, 24:D801, 17:D807, 17:D808, 17:D809, 23:D812, 23:D802, 23:D801, 18:D809, 18:D808, 18:D807, 22:D801, 22:D802, 22:D812, 23:D809, 23:D808, 23:D807, 22:D809, 22:D808, 22:D807, 21:D807, 21:D808, 21:D809, 21:D812, 21:D802, 21:D801, 20:D807, 20:D808, 20:D809, 19:D807, 19:D808, 19:D809, 20:D812, 20:D802, 20:D801, 1:D807, 1:D808, 1:D809, 2:D807, 2:D808, 2:D809, 1:D812, 1:D802, 1:D801, 2:D802, 2:D801, 2:D812, 3:D809, 3:D812, 3:D802, 3:D801, 4:D812, 4:D802, 4:D801, 5:D812, 5:D802, 5:D801, 6:D802, 6:D801, 6:D812, 7:D809, 7:D802, 7:D801, 7:D812, 8:D809, 8:D808, 8:D807, 14:D802, 14:D801, 14:D812, 13:D809, 13:D808, 13:D807, 27:D801, 27:D802, 27:D812, 28:D812, 28:D802, 28:D801, 29:D812, 29:D802, 29:D801, 12:D807, 12:D808, 12:D809, 13:D812, 13:D802, 13:D801, 9:D807, 9:D808, 9:D809, 8:D812, 8:D802, 8:D801, 9:D802, 9:D801, 9:D812, 10:D802, 10:D801, 10:D812, 10:D809, 10:D808, 10:D807, 12:D801, 12:D802, 12:D812, 11:D802, 11:D801, 11:D812, 11:D809, 11:D808, 11:D807, 30:D801, 30:D802, 30:D812, 30:D809, 30:D808, 30:D807, 29:D809, 29:D808, 29:D807, 28:D809, 28:D808, 28:D807, 27:D807, 27:D808, 27:D809, 26:D812, 26:D802, 26:D801, 14:D807, 14:D808, 14:D809, 15:D807, 15:D808, 15:D809, 15:D812, 15:D802, 15:D801, 7:D807, 7:D808, 6:D809, 6:D808, 6:D807, 16:D801, 16:D802, 16:D812, 5:D807, 5:D808, 5:D809, 4:D809, 3:D808, 3:D807, 19:D802, 19:D801, 19:D812, 18:D812, 18:D802, 18:D801, 4:D808, 4:D807, 17:D801, 17:D802, 17:D812, 16:D809, 16:D808, 16:D807, 25:D802, 25:D801, 25:D812, 26:D809, 26:D808, 26:D807, 25:D809, 25:D808, 25:D807,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">3- 22    </x:t>
-  </x:si>
-  <x:si>
     <x:t>2:D810, 2:D800, 12:D814, 12:D804, 12:D803, 12:D810, 12:D800, 22:D814, 22:D804, 22:D803, 23:D814, 23:D804, 23:D803, 23:D810, 23:D800, 22:D800, 22:D810, 21:D800, 21:D810, 21:D803, 21:D804, 21:D814, 11:D800, 11:D810, 11:D803, 11:D804, 11:D814, 1:D800, 1:D810, 1:D803, 1:D804, 1:D814, 2:D814, 2:D804, 2:D803, 3:D814, 3:D804, 3:D803, 4:D814, 4:D804, 4:D803, 5:D810, 5:D800, 6:D810, 5:D803, 5:D804, 5:D814, 6:D814, 6:D804, 6:D803, 7:D810, 6:D800, 16:D814, 16:D804, 16:D803, 16:D810, 16:D800, 27:D803, 27:D804, 27:D814, 17:D800, 17:D810, 17:D803, 17:D804, 17:D814, 7:D800, 8:D810, 7:D803, 7:D804, 7:D814, 8:D814, 8:D804, 8:D803, 9:D814, 9:D804, 9:D803, 10:D814, 10:D804, 10:D803, 10:D810, 10:D800, 20:D814, 20:D804, 20:D803, 20:D810, 20:D800, 30:D814, 30:D804, 30:D803, 30:D810, 30:D800, 29:D800, 29:D810, 29:D803, 29:D804, 29:D814, 19:D800, 19:D810, 19:D803, 19:D804, 19:D814, 9:D800, 9:D810, 8:D800, 18:D814, 18:D804, 18:D803, 18:D810, 18:D800, 28:D814, 28:D804, 28:D803, 28:D810, 28:D800, 27:D800, 27:D810, 26:D800, 26:D810, 26:D803, 26:D804, 26:D814, 25:D803, 25:D804, 25:D814, 15:D800, 15:D810, 15:D803, 15:D804, 15:D814, 14:D803, 14:D804, 14:D814, 4:D800, 4:D810, 3:D810, 3:D800, 13:D814, 13:D804, 13:D803, 13:D810, 13:D800, 14:D810, 14:D800, 24:D814, 24:D804, 24:D803, 24:D810, 24:D800, 25:D810, 25:D800,</x:t>
   </x:si>
   <x:si>
-    <x:t>06S2222001-24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30306S2222001-24</x:t>
-  </x:si>
-  <x:si>
     <x:t>30:Q803, 29:Q803, 28:Q803, 27:Q803, 26:Q803, 25:Q803, 24:Q803, 23:Q803, 22:Q803, 21:Q803, 15:Q803, 26:Q805, 26:Q802, 26:Q806, 17:Q803, 28:Q805, 28:Q802, 28:Q806, 19:Q803, 30:Q805, 30:Q802, 30:Q806, 20:Q803, 29:Q806, 29:Q802, 29:Q805, 18:Q803, 27:Q806, 27:Q802, 27:Q805, 16:Q803, 25:Q806, 25:Q802, 25:Q805, 14:Q803, 24:Q806, 24:Q802, 24:Q805, 13:Q803, 23:Q806, 23:Q802, 23:Q805, 12:Q803, 22:Q805, 22:Q806, 22:Q802, 21:Q806, 21:Q802, 21:Q805, 11:Q803, 11:Q806, 11:Q802, 11:Q805, 1:Q803, 12:Q805, 12:Q802, 12:Q806, 2:Q803, 13:Q805, 13:Q802, 13:Q806, 3:Q803, 14:Q805, 14:Q802, 14:Q806, 4:Q803, 15:Q805, 15:Q802, 15:Q806, 5:Q803, 16:Q805, 16:Q802, 16:Q806, 6:Q803, 17:Q805, 17:Q802, 17:Q806, 7:Q803, 18:Q805, 18:Q802, 18:Q806, 8:Q803, 19:Q805, 19:Q802, 19:Q806, 9:Q803, 20:Q805, 20:Q802, 20:Q806, 10:Q803, 10:Q806, 10:Q802, 10:Q805, 9:Q806, 9:Q802, 9:Q805, 8:Q806, 8:Q802, 8:Q805, 7:Q806, 7:Q802, 7:Q805, 6:Q806, 6:Q802, 6:Q805, 5:Q806, 5:Q802, 5:Q805, 4:Q806, 4:Q802, 4:Q805, 3:Q806, 3:Q802, 3:Q805, 2:Q806, 2:Q802, 2:Q805, 1:Q806, 1:Q802, 1:Q805,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">3- 23    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:Q808, 10:Q809, 9:Q808, 9:Q809, 8:Q808, 8:Q809, 7:Q808, 7:Q809, 6:Q808, 6:Q809, 5:Q808, 5:Q809, 4:Q808, 4:Q809, 3:Q808, 3:Q809, 2:Q808, 2:Q809, 1:Q808, 1:Q809, 20:Q809, 20:Q808, 19:Q809, 19:Q808, 18:Q809, 18:Q808, 17:Q809, 17:Q808, 16:Q809, 16:Q808, 15:Q809, 15:Q808, 14:Q809, 14:Q808, 13:Q809, 13:Q808, 12:Q809, 12:Q808, 11:Q809, 11:Q808, 30:Q808, 30:Q809, 29:Q808, 29:Q809, 28:Q808, 28:Q809, 27:Q808, 27:Q809, 26:Q808, 26:Q809, 25:Q808, 25:Q809, 24:Q808, 24:Q809, 23:Q808, 23:Q809, 22:Q808, 22:Q809, 21:Q808, 21:Q809,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>02S1040530-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30302S1040530-00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:C811, 9:C811, 8:C811, 7:C811, 6:C811, 5:C811, 4:C811, 3:C811, 2:C811, 1:C811, 20:C811, 19:C811, 18:C811, 17:C811, 16:C811, 15:C811, 14:C811, 13:C811, 12:C811, 11:C811, 30:C811, 29:C811, 28:C811, 27:C811, 26:C811, 25:C811, 24:C811, 23:C811, 22:C811, 21:C811,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">3- 24    </x:t>
-  </x:si>
-  <x:si>
     <x:t>1:C809, 1:C810, 1:C801, 1:C802, 11:C809, 11:C810, 11:C801, 11:C802, 21:C809, 21:C810, 21:C802, 21:C801, 22:C802, 22:C801, 22:C810, 22:C809, 23:C802, 23:C801, 23:C810, 23:C809, 24:C802, 24:C801, 24:C810, 24:C809, 25:C802, 25:C801, 25:C810, 25:C809, 26:C802, 26:C801, 26:C810, 26:C809, 27:C802, 27:C801, 27:C810, 27:C809, 28:C802, 28:C801, 28:C810, 28:C809, 29:C802, 29:C801, 29:C810, 29:C809, 30:C802, 30:C801, 30:C810, 30:C809, 20:C802, 20:C801, 20:C810, 20:C809, 10:C802, 10:C801, 10:C810, 10:C809, 9:C809, 9:C810, 8:C809, 8:C810, 7:C809, 7:C810, 6:C809, 6:C810, 5:C809, 5:C810, 4:C809, 4:C810, 3:C809, 3:C810, 2:C809, 2:C810, 2:C802, 2:C801, 3:C802, 3:C801, 4:C802, 4:C801, 5:C802, 5:C801, 6:C802, 6:C801, 7:C802, 7:C801, 8:C802, 8:C801, 9:C802, 9:C801, 19:C809, 19:C810, 19:C801, 19:C802, 18:C801, 18:C802, 17:C801, 17:C802, 16:C801, 16:C802, 15:C801, 15:C802, 14:C801, 14:C802, 13:C801, 13:C802, 12:C801, 12:C802, 12:C810, 12:C809, 13:C810, 13:C809, 14:C810, 14:C809, 15:C810, 15:C809, 16:C810, 16:C809, 17:C810, 17:C809, 18:C810, 18:C809,</x:t>
   </x:si>
   <x:si>
@@ -629,69 +743,9 @@
     <x:t xml:space="preserve">3- 26    </x:t>
   </x:si>
   <x:si>
-    <x:t>06S2907001-24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30306S2907001-24</x:t>
-  </x:si>
-  <x:si>
     <x:t>1:Q804, 2:Q804, 3:Q804, 4:Q804, 5:Q804, 6:Q804, 7:Q804, 8:Q804, 9:Q804, 10:Q804, 10:Q801, 20:Q804, 9:Q801, 19:Q804, 8:Q801, 18:Q804, 7:Q801, 17:Q804, 6:Q801, 16:Q804, 5:Q801, 15:Q804, 4:Q801, 14:Q804, 3:Q801, 13:Q804, 2:Q801, 12:Q804, 1:Q801, 11:Q804, 12:Q801, 23:Q804, 13:Q801, 24:Q804, 14:Q801, 25:Q804, 15:Q801, 26:Q804, 16:Q801, 27:Q804, 17:Q801, 28:Q804, 18:Q801, 29:Q804, 19:Q801, 20:Q801, 30:Q804, 30:Q801, 29:Q801, 28:Q801, 27:Q801, 26:Q801, 25:Q801, 24:Q801, 23:Q801, 22:Q804, 11:Q801, 21:Q804, 22:Q801, 21:Q801,</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">3- 28    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:Q810, 9:Q810, 8:Q810, 7:Q810, 6:Q810, 5:Q810, 4:Q810, 3:Q810, 2:Q810, 1:Q810, 20:Q810, 19:Q810, 18:Q810, 17:Q810, 16:Q810, 15:Q810, 14:Q810, 13:Q810, 12:Q810, 11:Q810, 30:Q810, 29:Q810, 28:Q810, 27:Q810, 26:Q810, 25:Q810, 24:Q810, 23:Q810, 22:Q810, 21:Q810,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>04S2206201-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30304S2206201-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:TVS800, 9:TVS800, 8:TVS800, 7:TVS800, 6:TVS800, 5:TVS800, 4:TVS800, 3:TVS800, 2:TVS800, 1:TVS800, 20:TVS800, 19:TVS800, 18:TVS800, 17:TVS800, 16:TVS800, 15:TVS800, 14:TVS800, 13:TVS800, 12:TVS800, 11:TVS800, 30:TVS800, 29:TVS800, 28:TVS800, 27:TVS800, 26:TVS800, 25:TVS800, 24:TVS800, 23:TVS800, 22:TVS800, 21:TVS800,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KT-1200F-180</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">3- 30    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>07S5190001-50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30307S5190001-50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30:U802, 29:U802, 28:U802, 27:U802, 26:U802, 25:U802, 24:U802, 23:U802, 22:U802, 21:U802, 20:U802, 19:U802, 18:U802, 17:U802, 16:U802, 15:U802, 14:U802, 13:U802, 12:U802, 11:U802, 10:U802, 9:U802, 8:U802, 7:U802, 6:U802, 5:U802, 4:U802, 3:U802, 2:U802, 1:U802,</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KT-1600F-380</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4- 11    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">11   </x:t>
-  </x:si>
-  <x:si>
-    <x:t>05S2100001-06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30305S2100001-06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:D811, 9:D811, 8:D811, 7:D811, 6:D811, 5:D811, 4:D811, 3:D811, 2:D811, 1:D811, 20:D811, 19:D811, 18:D811, 17:D811, 16:D811, 15:D811, 14:D811, 13:D811, 12:D811, 11:D811, 30:D811, 29:D811, 28:D811, 27:D811, 26:D811, 25:D811, 24:D811, 23:D811, 22:D811, 21:D811,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4- 14    </x:t>
-  </x:si>
-  <x:si>
     <x:t>05S3181000-18</x:t>
   </x:si>
   <x:si>
@@ -704,30 +758,6 @@
     <x:t xml:space="preserve">4- 18    </x:t>
   </x:si>
   <x:si>
-    <x:t>05SGU1M000-03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30305SGU1M000-03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:D806, 10:D805, 9:D806, 9:D805, 8:D806, 8:D805, 7:D806, 7:D805, 6:D806, 6:D805, 5:D806, 5:D805, 4:D806, 4:D805, 3:D806, 3:D805, 2:D806, 2:D805, 1:D806, 1:D805, 20:D805, 20:D806, 19:D805, 19:D806, 18:D805, 18:D806, 17:D805, 17:D806, 16:D805, 16:D806, 15:D805, 15:D806, 14:D805, 14:D806, 13:D805, 13:D806, 12:D805, 12:D806, 11:D805, 11:D806, 30:D806, 30:D805, 29:D806, 29:D805, 28:D806, 28:D805, 27:D806, 27:D805, 26:D806, 26:D805, 25:D806, 25:D805, 24:D806, 24:D805, 23:D806, 23:D805, 22:D806, 22:D805, 21:D806, 21:D805,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4- 23    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>07C8170003-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30307C8170003-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:U800, 10:U803, 9:U800, 9:U803, 8:U800, 8:U803, 7:U800, 7:U803, 6:U800, 6:U803, 5:U800, 5:U803, 4:U800, 4:U803, 3:U800, 3:U803, 2:U800, 2:U803, 1:U800, 1:U803, 20:U803, 20:U800, 19:U803, 19:U800, 18:U803, 18:U800, 17:U803, 17:U800, 16:U803, 16:U800, 15:U803, 15:U800, 14:U803, 14:U800, 13:U803, 13:U800, 12:U803, 12:U800, 11:U803, 11:U800, 30:U800, 30:U803, 29:U800, 29:U803, 28:U800, 28:U803, 27:U800, 27:U803, 26:U800, 26:U803, 25:U800, 25:U803, 24:U800, 24:U803, 23:U800, 23:U803, 22:U800, 22:U803, 21:U800, 21:U803,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4- 30    </x:t>
-  </x:si>
-  <x:si>
     <x:t>07S3930001-49</x:t>
   </x:si>
   <x:si>
@@ -740,21 +770,6 @@
     <x:t xml:space="preserve">4- 32    </x:t>
   </x:si>
   <x:si>
-    <x:t>04S2516101-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30304S2516101-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:TVS801, 9:TVS801, 8:TVS801, 7:TVS801, 6:TVS801, 5:TVS801, 4:TVS801, 3:TVS801, 2:TVS801, 1:TVS801, 20:TVS801, 19:TVS801, 18:TVS801, 17:TVS801, 16:TVS801, 15:TVS801, 14:TVS801, 13:TVS801, 12:TVS801, 11:TVS801, 30:TVS801, 29:TVS801, 28:TVS801, 27:TVS801, 26:TVS801, 25:TVS801, 24:TVS801, 23:TVS801, 22:TVS801, 21:TVS801,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4- 36    </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">36   </x:t>
-  </x:si>
-  <x:si>
     <x:t>06S5616001-20</x:t>
   </x:si>
   <x:si>
@@ -792,21 +807,6 @@
   </x:si>
   <x:si>
     <x:t>30:C812, 30:C800, 29:C812, 29:C800, 28:C812, 28:C800, 27:C812, 27:C800, 26:C812, 26:C800, 25:C812, 25:C800, 24:C812, 24:C800, 23:C812, 23:C800, 22:C812, 22:C800, 21:C800, 21:C812, 11:C800, 11:C812, 12:C800, 12:C812, 13:C800, 13:C812, 14:C800, 14:C812, 15:C800, 15:C812, 16:C800, 16:C812, 17:C800, 17:C812, 18:C800, 18:C812, 19:C800, 19:C812, 20:C800, 20:C812, 10:C800, 10:C812, 9:C812, 9:C800, 8:C812, 8:C800, 7:C812, 7:C800, 6:C812, 6:C800, 5:C812, 5:C800, 4:C812, 4:C800, 3:C812, 3:C800, 2:C812, 2:C800, 1:C812, 1:C800,</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">4- 8     </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">8    </x:t>
-  </x:si>
-  <x:si>
-    <x:t>07S7600301-50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MX2CDCCAQ600C00-F30307S7600301-50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30:U805, 29:U805, 28:U805, 27:U805, 26:U805, 25:U805, 24:U805, 23:U805, 22:U805, 21:U805, 20:U805, 19:U805, 18:U805, 17:U805, 16:U805, 15:U805, 14:U805, 13:U805, 12:U805, 11:U805, 10:U805, 9:U805, 8:U805, 7:U805, 6:U805, 5:U805, 4:U805, 3:U805, 2:U805, 1:U805,</x:t>
   </x:si>
   <x:si>
     <x:t>03S3216001-09</x:t>
@@ -906,7 +906,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="R6a555d4e92a74246" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="R8eecbc738a924337" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1318,7 +1318,7 @@
     </x:row>
     <x:row r="13" s="3" customFormat="1">
       <x:c r="A13" s="5">
-        <x:v>52541</x:v>
+        <x:v>52481</x:v>
       </x:c>
       <x:c r="B13" s="5" t="s">
         <x:v>4</x:v>
@@ -1342,24 +1342,24 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="I13" s="3" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J13" s="3" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="K13" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L13" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="Q13" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="14" s="3" customFormat="1">
       <x:c r="A14" s="5">
-        <x:v>52542</x:v>
+        <x:v>52482</x:v>
       </x:c>
       <x:c r="B14" s="5" t="s">
         <x:v>4</x:v>
@@ -1371,36 +1371,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E14" s="5" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F14" s="3" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="G14" s="3" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H14" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="I14" s="3" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="J14" s="3" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="K14" s="3" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="F14" s="3" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="G14" s="3" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="H14" s="3" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="I14" s="3" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="J14" s="3" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="K14" s="3" t="s">
-        <x:v>26</x:v>
-      </x:c>
       <x:c r="L14" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="Q14" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="15" s="3" customFormat="1">
       <x:c r="A15" s="5">
-        <x:v>52512</x:v>
+        <x:v>52483</x:v>
       </x:c>
       <x:c r="B15" s="5" t="s">
         <x:v>4</x:v>
@@ -1412,36 +1412,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E15" s="5" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F15" s="3" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="G15" s="3" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="H15" s="3" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="I15" s="3" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="J15" s="3" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="K15" s="3" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="L15" s="3" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="Q15" s="3" t="s">
         <x:v>32</x:v>
-      </x:c>
-      <x:c r="F15" s="3" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="G15" s="3" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="H15" s="3" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="I15" s="3" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="J15" s="3" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="K15" s="3" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="L15" s="3" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="Q15" s="3" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="16" s="3" customFormat="1">
       <x:c r="A16" s="5">
-        <x:v>52513</x:v>
+        <x:v>52484</x:v>
       </x:c>
       <x:c r="B16" s="5" t="s">
         <x:v>4</x:v>
@@ -1453,36 +1453,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E16" s="5" t="s">
-        <x:v>40</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F16" s="3" t="s">
-        <x:v>41</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G16" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H16" s="3" t="s">
-        <x:v>43</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="I16" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J16" s="3" t="s">
-        <x:v>44</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="K16" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L16" s="3" t="s">
-        <x:v>45</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Q16" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="17" s="3" customFormat="1">
       <x:c r="A17" s="5">
-        <x:v>52514</x:v>
+        <x:v>52485</x:v>
       </x:c>
       <x:c r="B17" s="5" t="s">
         <x:v>4</x:v>
@@ -1494,36 +1494,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E17" s="5" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F17" s="3" t="s">
-        <x:v>47</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="G17" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="H17" s="3" t="s">
-        <x:v>48</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="I17" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J17" s="3" t="s">
-        <x:v>49</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="K17" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L17" s="3" t="s">
-        <x:v>50</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="Q17" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="18" s="3" customFormat="1">
       <x:c r="A18" s="5">
-        <x:v>52481</x:v>
+        <x:v>52486</x:v>
       </x:c>
       <x:c r="B18" s="5" t="s">
         <x:v>4</x:v>
@@ -1535,36 +1535,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E18" s="5" t="s">
-        <x:v>46</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F18" s="3" t="s">
-        <x:v>47</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G18" s="3" t="s">
-        <x:v>51</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H18" s="3" t="s">
-        <x:v>52</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="I18" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J18" s="3" t="s">
-        <x:v>49</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="K18" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L18" s="3" t="s">
-        <x:v>50</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="Q18" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="19" s="3" customFormat="1">
       <x:c r="A19" s="5">
-        <x:v>52482</x:v>
+        <x:v>52487</x:v>
       </x:c>
       <x:c r="B19" s="5" t="s">
         <x:v>4</x:v>
@@ -1576,36 +1576,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E19" s="5" t="s">
-        <x:v>54</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F19" s="3" t="s">
-        <x:v>55</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="G19" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H19" s="3" t="s">
-        <x:v>57</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="I19" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J19" s="3" t="s">
-        <x:v>58</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="K19" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L19" s="3" t="s">
-        <x:v>59</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="Q19" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="20" s="3" customFormat="1">
       <x:c r="A20" s="5">
-        <x:v>52515</x:v>
+        <x:v>52488</x:v>
       </x:c>
       <x:c r="B20" s="5" t="s">
         <x:v>4</x:v>
@@ -1617,36 +1617,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E20" s="5" t="s">
-        <x:v>54</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F20" s="3" t="s">
-        <x:v>55</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G20" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H20" s="3" t="s">
-        <x:v>60</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="I20" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J20" s="3" t="s">
-        <x:v>58</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="K20" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L20" s="3" t="s">
-        <x:v>59</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="Q20" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="21" s="3" customFormat="1">
       <x:c r="A21" s="5">
-        <x:v>52516</x:v>
+        <x:v>52489</x:v>
       </x:c>
       <x:c r="B21" s="5" t="s">
         <x:v>4</x:v>
@@ -1658,36 +1658,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E21" s="5" t="s">
-        <x:v>61</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F21" s="3" t="s">
-        <x:v>62</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G21" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H21" s="3" t="s">
-        <x:v>63</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="I21" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J21" s="3" t="s">
-        <x:v>64</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="K21" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L21" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="Q21" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="22" s="3" customFormat="1">
       <x:c r="A22" s="5">
-        <x:v>52483</x:v>
+        <x:v>52490</x:v>
       </x:c>
       <x:c r="B22" s="5" t="s">
         <x:v>4</x:v>
@@ -1699,36 +1699,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E22" s="5" t="s">
-        <x:v>61</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F22" s="3" t="s">
-        <x:v>62</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G22" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="H22" s="3" t="s">
-        <x:v>66</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="I22" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J22" s="3" t="s">
-        <x:v>64</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K22" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L22" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="Q22" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="23" s="3" customFormat="1">
       <x:c r="A23" s="5">
-        <x:v>52517</x:v>
+        <x:v>52491</x:v>
       </x:c>
       <x:c r="B23" s="5" t="s">
         <x:v>4</x:v>
@@ -1740,36 +1740,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E23" s="5" t="s">
-        <x:v>67</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F23" s="3" t="s">
-        <x:v>68</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G23" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="H23" s="3" t="s">
-        <x:v>69</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="I23" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J23" s="3" t="s">
-        <x:v>70</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="K23" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L23" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Q23" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="24" s="3" customFormat="1">
       <x:c r="A24" s="5">
-        <x:v>52484</x:v>
+        <x:v>52492</x:v>
       </x:c>
       <x:c r="B24" s="5" t="s">
         <x:v>4</x:v>
@@ -1781,36 +1781,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E24" s="5" t="s">
-        <x:v>72</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F24" s="3" t="s">
-        <x:v>73</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G24" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="H24" s="3" t="s">
-        <x:v>74</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="I24" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J24" s="3" t="s">
-        <x:v>75</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="K24" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L24" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="Q24" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="25" s="3" customFormat="1">
       <x:c r="A25" s="5">
-        <x:v>52485</x:v>
+        <x:v>52493</x:v>
       </x:c>
       <x:c r="B25" s="5" t="s">
         <x:v>4</x:v>
@@ -1822,36 +1822,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E25" s="5" t="s">
-        <x:v>77</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="F25" s="3" t="s">
-        <x:v>78</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="G25" s="3" t="s">
-        <x:v>79</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H25" s="3" t="s">
-        <x:v>80</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I25" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J25" s="3" t="s">
-        <x:v>81</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="K25" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L25" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="Q25" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="26" s="3" customFormat="1">
       <x:c r="A26" s="5">
-        <x:v>52518</x:v>
+        <x:v>52494</x:v>
       </x:c>
       <x:c r="B26" s="5" t="s">
         <x:v>4</x:v>
@@ -1863,36 +1863,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E26" s="5" t="s">
-        <x:v>77</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F26" s="3" t="s">
-        <x:v>78</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="G26" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H26" s="3" t="s">
-        <x:v>83</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="I26" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J26" s="3" t="s">
-        <x:v>81</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="K26" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L26" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="Q26" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="27" s="3" customFormat="1">
       <x:c r="A27" s="5">
-        <x:v>52519</x:v>
+        <x:v>52495</x:v>
       </x:c>
       <x:c r="B27" s="5" t="s">
         <x:v>4</x:v>
@@ -1904,36 +1904,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E27" s="5" t="s">
-        <x:v>84</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="F27" s="3" t="s">
-        <x:v>85</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="G27" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H27" s="3" t="s">
-        <x:v>86</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="I27" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J27" s="3" t="s">
-        <x:v>87</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="K27" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L27" s="3" t="s">
-        <x:v>88</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="Q27" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="28" s="3" customFormat="1">
       <x:c r="A28" s="5">
-        <x:v>52486</x:v>
+        <x:v>52496</x:v>
       </x:c>
       <x:c r="B28" s="5" t="s">
         <x:v>4</x:v>
@@ -1945,36 +1945,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E28" s="5" t="s">
-        <x:v>84</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="F28" s="3" t="s">
-        <x:v>85</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="G28" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H28" s="3" t="s">
-        <x:v>89</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="I28" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J28" s="3" t="s">
-        <x:v>87</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="K28" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L28" s="3" t="s">
-        <x:v>88</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="Q28" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="29" s="3" customFormat="1">
       <x:c r="A29" s="5">
-        <x:v>52520</x:v>
+        <x:v>52497</x:v>
       </x:c>
       <x:c r="B29" s="5" t="s">
         <x:v>4</x:v>
@@ -1986,36 +1986,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E29" s="5" t="s">
-        <x:v>90</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F29" s="3" t="s">
-        <x:v>91</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="G29" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H29" s="3" t="s">
-        <x:v>92</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="I29" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J29" s="3" t="s">
-        <x:v>93</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="K29" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L29" s="3" t="s">
-        <x:v>94</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="Q29" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="30" s="3" customFormat="1">
       <x:c r="A30" s="5">
-        <x:v>52521</x:v>
+        <x:v>52498</x:v>
       </x:c>
       <x:c r="B30" s="5" t="s">
         <x:v>4</x:v>
@@ -2027,36 +2027,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E30" s="5" t="s">
-        <x:v>95</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F30" s="3" t="s">
-        <x:v>96</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="G30" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H30" s="3" t="s">
-        <x:v>97</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="I30" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J30" s="3" t="s">
-        <x:v>98</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="K30" s="3" t="s">
-        <x:v>38</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L30" s="3" t="s">
-        <x:v>99</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="Q30" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="31" s="3" customFormat="1">
       <x:c r="A31" s="5">
-        <x:v>52522</x:v>
+        <x:v>52499</x:v>
       </x:c>
       <x:c r="B31" s="5" t="s">
         <x:v>4</x:v>
@@ -2068,36 +2068,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E31" s="5" t="s">
-        <x:v>100</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F31" s="3" t="s">
-        <x:v>101</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="G31" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H31" s="3" t="s">
-        <x:v>102</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="I31" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J31" s="3" t="s">
-        <x:v>103</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="K31" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L31" s="3" t="s">
-        <x:v>105</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="Q31" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="32" s="3" customFormat="1">
       <x:c r="A32" s="5">
-        <x:v>52487</x:v>
+        <x:v>52500</x:v>
       </x:c>
       <x:c r="B32" s="5" t="s">
         <x:v>4</x:v>
@@ -2109,36 +2109,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E32" s="5" t="s">
-        <x:v>106</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F32" s="3" t="s">
-        <x:v>107</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="G32" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H32" s="3" t="s">
-        <x:v>108</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="I32" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J32" s="3" t="s">
-        <x:v>109</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="K32" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L32" s="3" t="s">
-        <x:v>110</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="Q32" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="33" s="3" customFormat="1">
       <x:c r="A33" s="5">
-        <x:v>52523</x:v>
+        <x:v>52501</x:v>
       </x:c>
       <x:c r="B33" s="5" t="s">
         <x:v>4</x:v>
@@ -2150,36 +2150,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E33" s="5" t="s">
-        <x:v>111</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F33" s="3" t="s">
-        <x:v>112</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G33" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="H33" s="3" t="s">
-        <x:v>113</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="I33" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J33" s="3" t="s">
-        <x:v>114</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="K33" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L33" s="3" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="Q33" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="34" s="3" customFormat="1">
       <x:c r="A34" s="5">
-        <x:v>52524</x:v>
+        <x:v>52502</x:v>
       </x:c>
       <x:c r="B34" s="5" t="s">
         <x:v>4</x:v>
@@ -2191,36 +2191,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E34" s="5" t="s">
-        <x:v>115</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F34" s="3" t="s">
-        <x:v>116</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="G34" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H34" s="3" t="s">
-        <x:v>117</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="I34" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J34" s="3" t="s">
-        <x:v>118</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="K34" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L34" s="3" t="s">
-        <x:v>119</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="Q34" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="35" s="3" customFormat="1">
       <x:c r="A35" s="5">
-        <x:v>52488</x:v>
+        <x:v>52503</x:v>
       </x:c>
       <x:c r="B35" s="5" t="s">
         <x:v>4</x:v>
@@ -2232,36 +2232,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E35" s="5" t="s">
-        <x:v>120</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F35" s="3" t="s">
-        <x:v>121</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G35" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H35" s="3" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="I35" s="3" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="J35" s="3" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="K35" s="3" t="s">
         <x:v>122</x:v>
       </x:c>
-      <x:c r="I35" s="3" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="J35" s="3" t="s">
-        <x:v>123</x:v>
-      </x:c>
-      <x:c r="K35" s="3" t="s">
-        <x:v>104</x:v>
-      </x:c>
       <x:c r="L35" s="3" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Q35" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="36" s="3" customFormat="1">
       <x:c r="A36" s="5">
-        <x:v>52489</x:v>
+        <x:v>52504</x:v>
       </x:c>
       <x:c r="B36" s="5" t="s">
         <x:v>4</x:v>
@@ -2273,36 +2273,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E36" s="5" t="s">
-        <x:v>124</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F36" s="3" t="s">
-        <x:v>125</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G36" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H36" s="3" t="s">
-        <x:v>126</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="I36" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J36" s="3" t="s">
-        <x:v>127</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="K36" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L36" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="Q36" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="37" s="3" customFormat="1">
       <x:c r="A37" s="5">
-        <x:v>52525</x:v>
+        <x:v>52505</x:v>
       </x:c>
       <x:c r="B37" s="5" t="s">
         <x:v>4</x:v>
@@ -2314,36 +2314,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E37" s="5" t="s">
-        <x:v>124</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="F37" s="3" t="s">
-        <x:v>125</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="G37" s="3" t="s">
-        <x:v>128</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H37" s="3" t="s">
-        <x:v>129</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="I37" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="J37" s="3" t="s">
-        <x:v>127</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="K37" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L37" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="Q37" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="38" s="3" customFormat="1">
       <x:c r="A38" s="5">
-        <x:v>52526</x:v>
+        <x:v>52507</x:v>
       </x:c>
       <x:c r="B38" s="5" t="s">
         <x:v>4</x:v>
@@ -2355,36 +2355,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E38" s="5" t="s">
-        <x:v>130</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="F38" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="G38" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H38" s="3" t="s">
-        <x:v>132</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="I38" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="J38" s="3" t="s">
-        <x:v>133</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="K38" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L38" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="Q38" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="39" s="3" customFormat="1">
       <x:c r="A39" s="5">
-        <x:v>52490</x:v>
+        <x:v>52508</x:v>
       </x:c>
       <x:c r="B39" s="5" t="s">
         <x:v>4</x:v>
@@ -2396,36 +2396,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E39" s="5" t="s">
-        <x:v>130</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="F39" s="3" t="s">
-        <x:v>131</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="G39" s="3" t="s">
-        <x:v>128</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H39" s="3" t="s">
-        <x:v>134</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="I39" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J39" s="3" t="s">
-        <x:v>133</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="K39" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L39" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="Q39" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="40" s="3" customFormat="1">
       <x:c r="A40" s="5">
-        <x:v>52491</x:v>
+        <x:v>52509</x:v>
       </x:c>
       <x:c r="B40" s="5" t="s">
         <x:v>4</x:v>
@@ -2437,36 +2437,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E40" s="5" t="s">
-        <x:v>135</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="F40" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="G40" s="3" t="s">
-        <x:v>79</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H40" s="3" t="s">
-        <x:v>137</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="I40" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="J40" s="3" t="s">
-        <x:v>138</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="K40" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L40" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="Q40" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="41" s="3" customFormat="1">
       <x:c r="A41" s="5">
-        <x:v>52527</x:v>
+        <x:v>52510</x:v>
       </x:c>
       <x:c r="B41" s="5" t="s">
         <x:v>4</x:v>
@@ -2478,36 +2478,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E41" s="5" t="s">
-        <x:v>135</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="F41" s="3" t="s">
-        <x:v>136</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="G41" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H41" s="3" t="s">
-        <x:v>139</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="I41" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="J41" s="3" t="s">
-        <x:v>138</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="K41" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L41" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="Q41" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="42" s="3" customFormat="1">
       <x:c r="A42" s="5">
-        <x:v>52528</x:v>
+        <x:v>52511</x:v>
       </x:c>
       <x:c r="B42" s="5" t="s">
         <x:v>4</x:v>
@@ -2519,36 +2519,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E42" s="5" t="s">
-        <x:v>140</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="F42" s="3" t="s">
-        <x:v>141</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="G42" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H42" s="3" t="s">
-        <x:v>142</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="I42" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="J42" s="3" t="s">
-        <x:v>143</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="K42" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L42" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="Q42" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="43" s="3" customFormat="1">
       <x:c r="A43" s="5">
-        <x:v>52492</x:v>
+        <x:v>52506</x:v>
       </x:c>
       <x:c r="B43" s="5" t="s">
         <x:v>4</x:v>
@@ -2560,36 +2560,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E43" s="5" t="s">
-        <x:v>140</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="F43" s="3" t="s">
-        <x:v>141</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="G43" s="3" t="s">
-        <x:v>79</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H43" s="3" t="s">
-        <x:v>144</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="I43" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="J43" s="3" t="s">
-        <x:v>143</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="K43" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L43" s="3" t="s">
-        <x:v>82</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="Q43" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="44" s="3" customFormat="1">
       <x:c r="A44" s="5">
-        <x:v>52493</x:v>
+        <x:v>52541</x:v>
       </x:c>
       <x:c r="B44" s="5" t="s">
         <x:v>4</x:v>
@@ -2601,36 +2601,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E44" s="5" t="s">
-        <x:v>145</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="F44" s="3" t="s">
-        <x:v>146</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="G44" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="H44" s="3" t="s">
-        <x:v>147</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="I44" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="J44" s="3" t="s">
-        <x:v>148</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="K44" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="L44" s="3" t="s">
-        <x:v>94</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="Q44" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="45" s="3" customFormat="1">
       <x:c r="A45" s="5">
-        <x:v>52494</x:v>
+        <x:v>52542</x:v>
       </x:c>
       <x:c r="B45" s="5" t="s">
         <x:v>4</x:v>
@@ -2642,36 +2642,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E45" s="5" t="s">
-        <x:v>149</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="F45" s="3" t="s">
-        <x:v>150</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="G45" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="H45" s="3" t="s">
-        <x:v>151</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="I45" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="J45" s="3" t="s">
-        <x:v>152</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="K45" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="L45" s="3" t="s">
-        <x:v>99</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="Q45" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="46" s="3" customFormat="1">
       <x:c r="A46" s="5">
-        <x:v>52495</x:v>
+        <x:v>52512</x:v>
       </x:c>
       <x:c r="B46" s="5" t="s">
         <x:v>4</x:v>
@@ -2683,36 +2683,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E46" s="5" t="s">
-        <x:v>153</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="F46" s="3" t="s">
-        <x:v>154</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="G46" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H46" s="3" t="s">
-        <x:v>155</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="I46" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J46" s="3" t="s">
-        <x:v>156</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="K46" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L46" s="3" t="s">
-        <x:v>157</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="Q46" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="47" s="3" customFormat="1">
       <x:c r="A47" s="5">
-        <x:v>52496</x:v>
+        <x:v>52513</x:v>
       </x:c>
       <x:c r="B47" s="5" t="s">
         <x:v>4</x:v>
@@ -2724,36 +2724,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E47" s="5" t="s">
-        <x:v>158</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="F47" s="3" t="s">
-        <x:v>159</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="G47" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="H47" s="3" t="s">
-        <x:v>160</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="I47" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J47" s="3" t="s">
-        <x:v>161</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="K47" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L47" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="Q47" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="48" s="3" customFormat="1">
       <x:c r="A48" s="5">
-        <x:v>52497</x:v>
+        <x:v>52514</x:v>
       </x:c>
       <x:c r="B48" s="5" t="s">
         <x:v>4</x:v>
@@ -2765,36 +2765,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E48" s="5" t="s">
-        <x:v>162</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F48" s="3" t="s">
-        <x:v>163</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G48" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H48" s="3" t="s">
-        <x:v>164</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="I48" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J48" s="3" t="s">
-        <x:v>165</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="K48" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L48" s="3" t="s">
-        <x:v>166</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="Q48" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="49" s="3" customFormat="1">
       <x:c r="A49" s="5">
-        <x:v>52498</x:v>
+        <x:v>52515</x:v>
       </x:c>
       <x:c r="B49" s="5" t="s">
         <x:v>4</x:v>
@@ -2806,36 +2806,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E49" s="5" t="s">
-        <x:v>167</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F49" s="3" t="s">
-        <x:v>168</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G49" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H49" s="3" t="s">
-        <x:v>169</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="I49" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J49" s="3" t="s">
-        <x:v>170</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K49" s="3" t="s">
-        <x:v>104</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L49" s="3" t="s">
-        <x:v>171</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="Q49" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="50" s="3" customFormat="1">
       <x:c r="A50" s="5">
-        <x:v>52529</x:v>
+        <x:v>52516</x:v>
       </x:c>
       <x:c r="B50" s="5" t="s">
         <x:v>4</x:v>
@@ -2847,36 +2847,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E50" s="5" t="s">
-        <x:v>172</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="F50" s="3" t="s">
-        <x:v>173</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G50" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H50" s="3" t="s">
-        <x:v>174</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="I50" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J50" s="3" t="s">
-        <x:v>175</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="K50" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L50" s="3" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="Q50" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="51" s="3" customFormat="1">
       <x:c r="A51" s="5">
-        <x:v>52499</x:v>
+        <x:v>52517</x:v>
       </x:c>
       <x:c r="B51" s="5" t="s">
         <x:v>4</x:v>
@@ -2888,36 +2888,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E51" s="5" t="s">
-        <x:v>177</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="F51" s="3" t="s">
-        <x:v>178</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="G51" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H51" s="3" t="s">
-        <x:v>179</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="I51" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J51" s="3" t="s">
-        <x:v>180</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="K51" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L51" s="3" t="s">
-        <x:v>181</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="Q51" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="52" s="3" customFormat="1">
       <x:c r="A52" s="5">
-        <x:v>52500</x:v>
+        <x:v>52518</x:v>
       </x:c>
       <x:c r="B52" s="5" t="s">
         <x:v>4</x:v>
@@ -2929,36 +2929,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E52" s="5" t="s">
-        <x:v>182</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F52" s="3" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="G52" s="3" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="H52" s="3" t="s">
+        <x:v>204</x:v>
+      </x:c>
+      <x:c r="I52" s="3" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="J52" s="3" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="K52" s="3" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="L52" s="3" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="Q52" s="3" t="s">
         <x:v>183</x:v>
-      </x:c>
-      <x:c r="G52" s="3" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="H52" s="3" t="s">
-        <x:v>184</x:v>
-      </x:c>
-      <x:c r="I52" s="3" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="J52" s="3" t="s">
-        <x:v>185</x:v>
-      </x:c>
-      <x:c r="K52" s="3" t="s">
-        <x:v>176</x:v>
-      </x:c>
-      <x:c r="L52" s="3" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="Q52" s="3" t="s">
-        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="53" s="3" customFormat="1">
       <x:c r="A53" s="5">
-        <x:v>52501</x:v>
+        <x:v>52519</x:v>
       </x:c>
       <x:c r="B53" s="5" t="s">
         <x:v>4</x:v>
@@ -2970,36 +2970,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E53" s="5" t="s">
-        <x:v>186</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="F53" s="3" t="s">
-        <x:v>187</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="G53" s="3" t="s">
-        <x:v>128</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="H53" s="3" t="s">
-        <x:v>188</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="I53" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J53" s="3" t="s">
-        <x:v>189</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="K53" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L53" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="Q53" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="54" s="3" customFormat="1">
       <x:c r="A54" s="5">
-        <x:v>52530</x:v>
+        <x:v>52520</x:v>
       </x:c>
       <x:c r="B54" s="5" t="s">
         <x:v>4</x:v>
@@ -3011,36 +3011,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E54" s="5" t="s">
-        <x:v>186</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="F54" s="3" t="s">
-        <x:v>187</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="G54" s="3" t="s">
-        <x:v>51</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H54" s="3" t="s">
-        <x:v>190</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="I54" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J54" s="3" t="s">
-        <x:v>189</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="K54" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L54" s="3" t="s">
-        <x:v>65</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="Q54" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="55" s="3" customFormat="1">
       <x:c r="A55" s="5">
-        <x:v>52531</x:v>
+        <x:v>52521</x:v>
       </x:c>
       <x:c r="B55" s="5" t="s">
         <x:v>4</x:v>
@@ -3052,36 +3052,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E55" s="5" t="s">
-        <x:v>191</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="F55" s="3" t="s">
-        <x:v>192</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="G55" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H55" s="3" t="s">
-        <x:v>193</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="I55" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J55" s="3" t="s">
-        <x:v>194</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="K55" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="L55" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="Q55" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="56" s="3" customFormat="1">
       <x:c r="A56" s="5">
-        <x:v>52502</x:v>
+        <x:v>52522</x:v>
       </x:c>
       <x:c r="B56" s="5" t="s">
         <x:v>4</x:v>
@@ -3093,36 +3093,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E56" s="5" t="s">
-        <x:v>191</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="F56" s="3" t="s">
-        <x:v>192</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="G56" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H56" s="3" t="s">
-        <x:v>195</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="I56" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J56" s="3" t="s">
-        <x:v>194</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="K56" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L56" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="Q56" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="57" s="3" customFormat="1">
       <x:c r="A57" s="5">
-        <x:v>52503</x:v>
+        <x:v>52523</x:v>
       </x:c>
       <x:c r="B57" s="5" t="s">
         <x:v>4</x:v>
@@ -3134,36 +3134,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E57" s="5" t="s">
-        <x:v>196</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="F57" s="3" t="s">
-        <x:v>197</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="G57" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H57" s="3" t="s">
-        <x:v>198</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="I57" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J57" s="3" t="s">
-        <x:v>199</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="K57" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L57" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="Q57" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="58" s="3" customFormat="1">
       <x:c r="A58" s="5">
-        <x:v>52532</x:v>
+        <x:v>52524</x:v>
       </x:c>
       <x:c r="B58" s="5" t="s">
         <x:v>4</x:v>
@@ -3175,36 +3175,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E58" s="5" t="s">
-        <x:v>196</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="F58" s="3" t="s">
-        <x:v>197</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="G58" s="3" t="s">
-        <x:v>42</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H58" s="3" t="s">
-        <x:v>200</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="I58" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J58" s="3" t="s">
-        <x:v>199</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="K58" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L58" s="3" t="s">
-        <x:v>76</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="Q58" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="59" s="3" customFormat="1">
       <x:c r="A59" s="5">
-        <x:v>52533</x:v>
+        <x:v>52525</x:v>
       </x:c>
       <x:c r="B59" s="5" t="s">
         <x:v>4</x:v>
@@ -3216,36 +3216,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E59" s="5" t="s">
-        <x:v>201</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="F59" s="3" t="s">
-        <x:v>202</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="G59" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="H59" s="3" t="s">
-        <x:v>203</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="I59" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J59" s="3" t="s">
-        <x:v>204</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="K59" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L59" s="3" t="s">
-        <x:v>88</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="Q59" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="60" s="3" customFormat="1">
       <x:c r="A60" s="5">
-        <x:v>52534</x:v>
+        <x:v>52526</x:v>
       </x:c>
       <x:c r="B60" s="5" t="s">
         <x:v>4</x:v>
@@ -3257,36 +3257,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E60" s="5" t="s">
-        <x:v>205</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="F60" s="3" t="s">
-        <x:v>206</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="G60" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H60" s="3" t="s">
-        <x:v>207</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="I60" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J60" s="3" t="s">
-        <x:v>208</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K60" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L60" s="3" t="s">
-        <x:v>99</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="Q60" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="61" s="3" customFormat="1">
       <x:c r="A61" s="5">
-        <x:v>52504</x:v>
+        <x:v>52527</x:v>
       </x:c>
       <x:c r="B61" s="5" t="s">
         <x:v>4</x:v>
@@ -3298,36 +3298,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E61" s="5" t="s">
-        <x:v>205</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="F61" s="3" t="s">
-        <x:v>206</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="G61" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H61" s="3" t="s">
-        <x:v>209</x:v>
+        <x:v>230</x:v>
       </x:c>
       <x:c r="I61" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J61" s="3" t="s">
-        <x:v>208</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="K61" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L61" s="3" t="s">
-        <x:v>99</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Q61" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="62" s="3" customFormat="1">
       <x:c r="A62" s="5">
-        <x:v>52505</x:v>
+        <x:v>52528</x:v>
       </x:c>
       <x:c r="B62" s="5" t="s">
         <x:v>4</x:v>
@@ -3339,36 +3339,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E62" s="5" t="s">
-        <x:v>210</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F62" s="3" t="s">
-        <x:v>211</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="G62" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H62" s="3" t="s">
-        <x:v>212</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="I62" s="3" t="s">
-        <x:v>213</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J62" s="3" t="s">
-        <x:v>214</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="K62" s="3" t="s">
-        <x:v>176</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L62" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="Q62" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="63" s="3" customFormat="1">
       <x:c r="A63" s="5">
-        <x:v>52507</x:v>
+        <x:v>52529</x:v>
       </x:c>
       <x:c r="B63" s="5" t="s">
         <x:v>4</x:v>
@@ -3380,36 +3380,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E63" s="5" t="s">
-        <x:v>215</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="F63" s="3" t="s">
-        <x:v>216</x:v>
+        <x:v>233</x:v>
       </x:c>
       <x:c r="G63" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H63" s="3" t="s">
-        <x:v>217</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="I63" s="3" t="s">
-        <x:v>218</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J63" s="3" t="s">
-        <x:v>219</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="K63" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L63" s="3" t="s">
-        <x:v>221</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="Q63" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="64" s="3" customFormat="1">
       <x:c r="A64" s="5">
-        <x:v>52508</x:v>
+        <x:v>52530</x:v>
       </x:c>
       <x:c r="B64" s="5" t="s">
         <x:v>4</x:v>
@@ -3421,36 +3421,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E64" s="5" t="s">
-        <x:v>222</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F64" s="3" t="s">
-        <x:v>223</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="G64" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H64" s="3" t="s">
-        <x:v>224</x:v>
+        <x:v>236</x:v>
       </x:c>
       <x:c r="I64" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J64" s="3" t="s">
-        <x:v>225</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="K64" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L64" s="3" t="s">
-        <x:v>110</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="Q64" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="65" s="3" customFormat="1">
       <x:c r="A65" s="5">
-        <x:v>52538</x:v>
+        <x:v>52531</x:v>
       </x:c>
       <x:c r="B65" s="5" t="s">
         <x:v>4</x:v>
@@ -3462,36 +3462,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E65" s="5" t="s">
-        <x:v>226</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="F65" s="3" t="s">
-        <x:v>227</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="G65" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="H65" s="3" t="s">
-        <x:v>228</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="I65" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J65" s="3" t="s">
-        <x:v>229</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="K65" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L65" s="3" t="s">
-        <x:v>45</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="Q65" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="66" s="3" customFormat="1">
       <x:c r="A66" s="5">
-        <x:v>52509</x:v>
+        <x:v>52532</x:v>
       </x:c>
       <x:c r="B66" s="5" t="s">
         <x:v>4</x:v>
@@ -3503,36 +3503,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E66" s="5" t="s">
-        <x:v>230</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="F66" s="3" t="s">
-        <x:v>231</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="G66" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="H66" s="3" t="s">
-        <x:v>232</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="I66" s="3" t="s">
-        <x:v>213</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J66" s="3" t="s">
-        <x:v>233</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="K66" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L66" s="3" t="s">
-        <x:v>71</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="Q66" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="67" s="3" customFormat="1">
       <x:c r="A67" s="5">
-        <x:v>52510</x:v>
+        <x:v>52533</x:v>
       </x:c>
       <x:c r="B67" s="5" t="s">
         <x:v>4</x:v>
@@ -3544,36 +3544,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E67" s="5" t="s">
-        <x:v>234</x:v>
+        <x:v>239</x:v>
       </x:c>
       <x:c r="F67" s="3" t="s">
-        <x:v>235</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="G67" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H67" s="3" t="s">
-        <x:v>236</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="I67" s="3" t="s">
-        <x:v>218</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J67" s="3" t="s">
-        <x:v>237</x:v>
+        <x:v>242</x:v>
       </x:c>
       <x:c r="K67" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L67" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="Q67" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="68" s="3" customFormat="1">
       <x:c r="A68" s="5">
-        <x:v>52539</x:v>
+        <x:v>52534</x:v>
       </x:c>
       <x:c r="B68" s="5" t="s">
         <x:v>4</x:v>
@@ -3585,36 +3585,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E68" s="5" t="s">
-        <x:v>238</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="F68" s="3" t="s">
-        <x:v>239</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="G68" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H68" s="3" t="s">
-        <x:v>240</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="I68" s="3" t="s">
-        <x:v>213</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J68" s="3" t="s">
-        <x:v>241</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="K68" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="L68" s="3" t="s">
-        <x:v>171</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="Q68" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="69" s="3" customFormat="1">
       <x:c r="A69" s="5">
-        <x:v>52511</x:v>
+        <x:v>52538</x:v>
       </x:c>
       <x:c r="B69" s="5" t="s">
         <x:v>4</x:v>
@@ -3626,36 +3626,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E69" s="5" t="s">
-        <x:v>242</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="F69" s="3" t="s">
-        <x:v>243</x:v>
+        <x:v>245</x:v>
       </x:c>
       <x:c r="G69" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H69" s="3" t="s">
-        <x:v>244</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="I69" s="3" t="s">
-        <x:v>213</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J69" s="3" t="s">
-        <x:v>245</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="K69" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L69" s="3" t="s">
-        <x:v>246</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="Q69" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="70" s="3" customFormat="1">
       <x:c r="A70" s="5">
-        <x:v>52540</x:v>
+        <x:v>52539</x:v>
       </x:c>
       <x:c r="B70" s="5" t="s">
         <x:v>4</x:v>
@@ -3667,36 +3667,36 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="E70" s="5" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
       <x:c r="F70" s="3" t="s">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="G70" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H70" s="3" t="s">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="I70" s="3" t="s">
-        <x:v>213</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="J70" s="3" t="s">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
       <x:c r="K70" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L70" s="3" t="s">
-        <x:v>251</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="Q70" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="71" s="3" customFormat="1">
       <x:c r="A71" s="5">
-        <x:v>52535</x:v>
+        <x:v>52540</x:v>
       </x:c>
       <x:c r="B71" s="5" t="s">
         <x:v>4</x:v>
@@ -3714,30 +3714,30 @@
         <x:v>253</x:v>
       </x:c>
       <x:c r="G71" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H71" s="3" t="s">
         <x:v>254</x:v>
       </x:c>
       <x:c r="I71" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="J71" s="3" t="s">
         <x:v>255</x:v>
       </x:c>
       <x:c r="K71" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L71" s="3" t="s">
         <x:v>256</x:v>
       </x:c>
       <x:c r="Q71" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="72" s="3" customFormat="1">
       <x:c r="A72" s="5">
-        <x:v>52536</x:v>
+        <x:v>52535</x:v>
       </x:c>
       <x:c r="B72" s="5" t="s">
         <x:v>4</x:v>
@@ -3755,30 +3755,30 @@
         <x:v>258</x:v>
       </x:c>
       <x:c r="G72" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="H72" s="3" t="s">
         <x:v>259</x:v>
       </x:c>
       <x:c r="I72" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J72" s="3" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="K72" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L72" s="3" t="s">
         <x:v>261</x:v>
       </x:c>
       <x:c r="Q72" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="73" s="3" customFormat="1">
       <x:c r="A73" s="5">
-        <x:v>52506</x:v>
+        <x:v>52536</x:v>
       </x:c>
       <x:c r="B73" s="5" t="s">
         <x:v>4</x:v>
@@ -3796,25 +3796,25 @@
         <x:v>263</x:v>
       </x:c>
       <x:c r="G73" s="3" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H73" s="3" t="s">
         <x:v>264</x:v>
       </x:c>
       <x:c r="I73" s="3" t="s">
-        <x:v>218</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J73" s="3" t="s">
-        <x:v>260</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="K73" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L73" s="3" t="s">
-        <x:v>261</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="Q73" s="3" t="s">
-        <x:v>53</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
     <x:row r="74" s="3" customFormat="1">
@@ -3837,31 +3837,31 @@
         <x:v>266</x:v>
       </x:c>
       <x:c r="G74" s="3" t="s">
-        <x:v>56</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H74" s="3" t="s">
         <x:v>267</x:v>
       </x:c>
       <x:c r="I74" s="3" t="s">
-        <x:v>36</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="J74" s="3" t="s">
         <x:v>268</x:v>
       </x:c>
       <x:c r="K74" s="3" t="s">
-        <x:v>220</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="L74" s="3" t="s">
         <x:v>269</x:v>
       </x:c>
       <x:c r="Q74" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>183</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">
     <x:mergeCell ref="A2:E2"/>
   </x:mergeCells>
-  <x:drawing r:id="Rd2aef2b9f88a4664"/>
+  <x:drawing r:id="R9d2f81c0b1ed49db"/>
 </x:worksheet>
 </file>
</xml_diff>